<commit_message>
New algorithm and control
</commit_message>
<xml_diff>
--- a/FreescaleCup2013/testing/Algorithm_ORA/Algorithms.xlsx
+++ b/FreescaleCup2013/testing/Algorithm_ORA/Algorithms.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="NoDummy" sheetId="1" r:id="rId1"/>
+    <sheet name="Speeds" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Speed</t>
   </si>
@@ -47,21 +48,86 @@
     <t>Difference</t>
   </si>
   <si>
-    <t>diff/50</t>
-  </si>
-  <si>
     <t>(diff/35)^2</t>
   </si>
   <si>
     <t>(diff/40)^3</t>
+  </si>
+  <si>
+    <t>Algoritmo</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>vfnDiff_1</t>
+  </si>
+  <si>
+    <t>vfnSpeedsHard(coeff=0.2)</t>
+  </si>
+  <si>
+    <t>vfnSpeedsHard(coeff=0.12)</t>
+  </si>
+  <si>
+    <t>vfnSpeedsHard(coeff=0.3)</t>
+  </si>
+  <si>
+    <t>vfnSpeedsHard(coeff=0.35)</t>
+  </si>
+  <si>
+    <t>Misma velocidad en los 3 casos</t>
+  </si>
+  <si>
+    <t>Caracteristicas</t>
+  </si>
+  <si>
+    <t>Se sale mucho el carrito, recomendable a velocidades moderadas</t>
+  </si>
+  <si>
+    <t>velocidad cte, buenas vueltas</t>
+  </si>
+  <si>
+    <t>Orden</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Lap 1</t>
+  </si>
+  <si>
+    <t>Lap 2</t>
+  </si>
+  <si>
+    <t>Se frena en la curva, alcanza a derrapar</t>
+  </si>
+  <si>
+    <t>vfnDiff_2</t>
+  </si>
+  <si>
+    <t>diff/45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,10 +170,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -115,8 +190,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -382,157 +463,157 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
                 <c:pt idx="0">
-                  <c:v>-0.98</c:v>
+                  <c:v>-1.0888888888888888</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.94</c:v>
+                  <c:v>-1.0444444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.9</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.86</c:v>
+                  <c:v>-0.9555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.82</c:v>
+                  <c:v>-0.91111111111111109</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.78</c:v>
+                  <c:v>-0.8666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.74</c:v>
+                  <c:v>-0.82222222222222219</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.7</c:v>
+                  <c:v>-0.77777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.66</c:v>
+                  <c:v>-0.73333333333333328</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.62</c:v>
+                  <c:v>-0.68888888888888888</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.57999999999999996</c:v>
+                  <c:v>-0.64444444444444449</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.54</c:v>
+                  <c:v>-0.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.5</c:v>
+                  <c:v>-0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.46</c:v>
+                  <c:v>-0.51111111111111107</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.42</c:v>
+                  <c:v>-0.46666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.38</c:v>
+                  <c:v>-0.42222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.34</c:v>
+                  <c:v>-0.37777777777777777</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.3</c:v>
+                  <c:v>-0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.26</c:v>
+                  <c:v>-0.28888888888888886</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.22</c:v>
+                  <c:v>-0.24444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.18</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.14000000000000001</c:v>
+                  <c:v>-0.15555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.1</c:v>
+                  <c:v>-0.1111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.06</c:v>
+                  <c:v>-6.6666666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.02</c:v>
+                  <c:v>-2.2222222222222223E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.02</c:v>
+                  <c:v>2.2222222222222223E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.06</c:v>
+                  <c:v>6.6666666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.1</c:v>
+                  <c:v>0.1111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.15555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.18</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.22</c:v>
+                  <c:v>0.24444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.26</c:v>
+                  <c:v>0.28888888888888886</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.3</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.34</c:v>
+                  <c:v>0.37777777777777777</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.38</c:v>
+                  <c:v>0.42222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.42</c:v>
+                  <c:v>0.46666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.46</c:v>
+                  <c:v>0.51111111111111107</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.5</c:v>
+                  <c:v>0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.54</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.64444444444444449</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.62</c:v>
+                  <c:v>0.68888888888888888</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.66</c:v>
+                  <c:v>0.73333333333333328</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.7</c:v>
+                  <c:v>0.77777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.74</c:v>
+                  <c:v>0.82222222222222219</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.78</c:v>
+                  <c:v>0.8666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.82</c:v>
+                  <c:v>0.91111111111111109</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.86</c:v>
+                  <c:v>0.9555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.9</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.94</c:v>
+                  <c:v>1.0444444444444445</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.98</c:v>
+                  <c:v>1.0888888888888888</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1108,128 +1189,110 @@
                 <c:pt idx="4">
                   <c:v>-1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.92685937499999993</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.79145312500000009</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.669921875</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.56151562499999996</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.46548437500000006</c:v>
+                  <c:v>-0.82897849013551506</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.38107812499999999</c:v>
+                  <c:v>-0.67865987700698438</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.30754687500000005</c:v>
+                  <c:v>-0.54770848985725029</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.244140625</c:v>
+                  <c:v>-0.43478865792915378</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.19010937499999994</c:v>
+                  <c:v>-0.33856471046553699</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.14470312500000002</c:v>
+                  <c:v>-0.25770097670924114</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.10717187499999999</c:v>
+                  <c:v>-0.19086178590310826</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-7.676562499999999E-2</c:v>
+                  <c:v>-0.13671146728997968</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-5.2734375E-2</c:v>
+                  <c:v>-9.3914350112697206E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3.4328125000000008E-2</c:v>
+                  <c:v>-6.1134763614102451E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-2.0796875000000006E-2</c:v>
+                  <c:v>-3.7037037037037035E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.1390625000000001E-2</c:v>
+                  <c:v>-2.0285499624342593E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-5.3593749999999987E-3</c:v>
+                  <c:v>-9.5444806188607848E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-1.953125E-3</c:v>
+                  <c:v>-3.4783092634332307E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-4.21875E-4</c:v>
+                  <c:v>-7.513148009015778E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-1.5625000000000004E-5</c:v>
+                  <c:v>-2.7826474107465846E-5</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.5625000000000004E-5</c:v>
+                  <c:v>2.7826474107465846E-5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.21875E-4</c:v>
+                  <c:v>7.513148009015778E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.953125E-3</c:v>
+                  <c:v>3.4783092634332307E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>5.3593749999999987E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.1390625000000001E-2</c:v>
+                  <c:v>2.0285499624342593E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.0796875000000006E-2</c:v>
+                  <c:v>3.7037037037037035E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.4328125000000008E-2</c:v>
+                  <c:v>6.1134763614102451E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.2734375E-2</c:v>
+                  <c:v>9.3914350112697206E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.676562499999999E-2</c:v>
+                  <c:v>0.13671146728997968</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.10717187499999999</c:v>
+                  <c:v>0.19086178590310826</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.14470312500000002</c:v>
+                  <c:v>0.25770097670924114</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.19010937499999994</c:v>
+                  <c:v>0.33856471046553699</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.244140625</c:v>
+                  <c:v>0.43478865792915378</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.30754687500000005</c:v>
+                  <c:v>0.54770848985725029</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.38107812499999999</c:v>
+                  <c:v>0.67865987700698438</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.46548437500000006</c:v>
+                  <c:v>0.82897849013551506</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.56151562499999996</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.669921875</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.79145312500000009</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.92685937499999993</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>1</c:v>
@@ -1259,8 +1322,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="269093488"/>
-        <c:axId val="277450608"/>
+        <c:axId val="183750384"/>
+        <c:axId val="183750944"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1472,157 +1535,157 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="51"/>
                       <c:pt idx="0">
-                        <c:v>1.536</c:v>
+                        <c:v>1.612222222222222</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>1.508</c:v>
+                        <c:v>1.5811111111111111</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>1.48</c:v>
+                        <c:v>1.5499999999999998</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>1.452</c:v>
+                        <c:v>1.5188888888888887</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>1.4239999999999999</c:v>
+                        <c:v>1.4877777777777776</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.3959999999999999</c:v>
+                        <c:v>1.4566666666666666</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>1.3679999999999999</c:v>
+                        <c:v>1.4255555555555555</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.3399999999999999</c:v>
+                        <c:v>1.3944444444444444</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>1.3119999999999998</c:v>
+                        <c:v>1.3633333333333333</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>1.284</c:v>
+                        <c:v>1.3322222222222222</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1.256</c:v>
+                        <c:v>1.3011111111111111</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>1.228</c:v>
+                        <c:v>1.27</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>1.2</c:v>
+                        <c:v>1.2388888888888889</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1.1719999999999999</c:v>
+                        <c:v>1.2077777777777778</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1.1439999999999999</c:v>
+                        <c:v>1.1766666666666667</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>1.1159999999999999</c:v>
+                        <c:v>1.1455555555555554</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>1.0880000000000001</c:v>
+                        <c:v>1.1144444444444443</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>1.06</c:v>
+                        <c:v>1.0833333333333333</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>1.032</c:v>
+                        <c:v>1.0522222222222222</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>1.004</c:v>
+                        <c:v>1.0211111111111111</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>0.97599999999999998</c:v>
+                        <c:v>0.99</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>0.94799999999999995</c:v>
+                        <c:v>0.9588888888888889</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>0.91999999999999993</c:v>
+                        <c:v>0.9277777777777777</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>0.89200000000000002</c:v>
+                        <c:v>0.89666666666666661</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>0.86399999999999999</c:v>
+                        <c:v>0.86555555555555552</c:v>
                       </c:pt>
                       <c:pt idx="25">
                         <c:v>0.85</c:v>
                       </c:pt>
                       <c:pt idx="26">
-                        <c:v>0.83599999999999997</c:v>
+                        <c:v>0.83444444444444443</c:v>
                       </c:pt>
                       <c:pt idx="27">
-                        <c:v>0.80799999999999994</c:v>
+                        <c:v>0.80333333333333334</c:v>
                       </c:pt>
                       <c:pt idx="28">
-                        <c:v>0.78</c:v>
+                        <c:v>0.77222222222222225</c:v>
                       </c:pt>
                       <c:pt idx="29">
-                        <c:v>0.752</c:v>
+                        <c:v>0.74111111111111105</c:v>
                       </c:pt>
                       <c:pt idx="30">
-                        <c:v>0.72399999999999998</c:v>
+                        <c:v>0.71</c:v>
                       </c:pt>
                       <c:pt idx="31">
-                        <c:v>0.69599999999999995</c:v>
+                        <c:v>0.67888888888888888</c:v>
                       </c:pt>
                       <c:pt idx="32">
-                        <c:v>0.66799999999999993</c:v>
+                        <c:v>0.64777777777777779</c:v>
                       </c:pt>
                       <c:pt idx="33">
-                        <c:v>0.64</c:v>
+                        <c:v>0.6166666666666667</c:v>
                       </c:pt>
                       <c:pt idx="34">
-                        <c:v>0.61199999999999999</c:v>
+                        <c:v>0.58555555555555561</c:v>
                       </c:pt>
                       <c:pt idx="35">
-                        <c:v>0.58400000000000007</c:v>
+                        <c:v>0.55444444444444452</c:v>
                       </c:pt>
                       <c:pt idx="36">
-                        <c:v>0.55600000000000005</c:v>
+                        <c:v>0.52333333333333332</c:v>
                       </c:pt>
                       <c:pt idx="37">
-                        <c:v>0.52800000000000002</c:v>
+                        <c:v>0.49222222222222223</c:v>
                       </c:pt>
                       <c:pt idx="38">
-                        <c:v>0.5</c:v>
+                        <c:v>0.46111111111111108</c:v>
                       </c:pt>
                       <c:pt idx="39">
-                        <c:v>0.47199999999999998</c:v>
+                        <c:v>0.43</c:v>
                       </c:pt>
                       <c:pt idx="40">
-                        <c:v>0.44400000000000001</c:v>
+                        <c:v>0.39888888888888885</c:v>
                       </c:pt>
                       <c:pt idx="41">
-                        <c:v>0.41599999999999998</c:v>
+                        <c:v>0.36777777777777781</c:v>
                       </c:pt>
                       <c:pt idx="42">
-                        <c:v>0.38800000000000001</c:v>
+                        <c:v>0.33666666666666667</c:v>
                       </c:pt>
                       <c:pt idx="43">
-                        <c:v>0.36000000000000004</c:v>
+                        <c:v>0.30555555555555558</c:v>
                       </c:pt>
                       <c:pt idx="44">
-                        <c:v>0.33199999999999996</c:v>
+                        <c:v>0.27444444444444449</c:v>
                       </c:pt>
                       <c:pt idx="45">
-                        <c:v>0.30400000000000005</c:v>
+                        <c:v>0.24333333333333329</c:v>
                       </c:pt>
                       <c:pt idx="46">
-                        <c:v>0.27600000000000002</c:v>
+                        <c:v>0.2122222222222222</c:v>
                       </c:pt>
                       <c:pt idx="47">
-                        <c:v>0.248</c:v>
+                        <c:v>0.18111111111111111</c:v>
                       </c:pt>
                       <c:pt idx="48">
-                        <c:v>0.21999999999999997</c:v>
+                        <c:v>0.15000000000000002</c:v>
                       </c:pt>
                       <c:pt idx="49">
-                        <c:v>0.19200000000000006</c:v>
+                        <c:v>0.11888888888888882</c:v>
                       </c:pt>
                       <c:pt idx="50">
-                        <c:v>0.16400000000000003</c:v>
+                        <c:v>8.7777777777777843E-2</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1660,7 +1723,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>NoDummy!$A$10:$A$60</c15:sqref>
@@ -1828,7 +1891,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>NoDummy!$C$10:$C$60</c15:sqref>
@@ -1874,7 +1937,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>NoDummy!$A$10:$A$60</c15:sqref>
@@ -2042,7 +2105,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>NoDummy!$D$10:$D$60</c15:sqref>
@@ -2088,7 +2151,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>NoDummy!$A$10:$A$60</c15:sqref>
@@ -2256,7 +2319,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>NoDummy!$F$10:$F$60</c15:sqref>
@@ -2429,7 +2492,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="269093488"/>
+        <c:axId val="183750384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2486,12 +2549,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277450608"/>
+        <c:crossAx val="183750944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="277450608"/>
+        <c:axId val="183750944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2548,7 +2611,7 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="269093488"/>
+        <c:crossAx val="183750384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3157,16 +3220,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3453,8 +3516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3496,46 +3559,46 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="G5" s="3" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="G5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.7</v>
       </c>
       <c r="G7" s="1">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H7" s="1">
         <v>35</v>
       </c>
       <c r="I7" s="1">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3554,7 +3617,7 @@
       </c>
       <c r="B10" s="1">
         <f>(G10*-A7)+A8</f>
-        <v>1.536</v>
+        <v>1.612222222222222</v>
       </c>
       <c r="F10" s="1">
         <f>A10-63</f>
@@ -3562,7 +3625,7 @@
       </c>
       <c r="G10" s="1">
         <f>F10/G7</f>
-        <v>-0.98</v>
+        <v>-1.0888888888888888</v>
       </c>
       <c r="H10" s="1">
         <v>-1</v>
@@ -3577,7 +3640,7 @@
       </c>
       <c r="B11" s="1">
         <f>(G11*-A7)+A8</f>
-        <v>1.508</v>
+        <v>1.5811111111111111</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" ref="F11:F60" si="0">A11-63</f>
@@ -3585,7 +3648,7 @@
       </c>
       <c r="G11" s="1">
         <f>F11/G7</f>
-        <v>-0.94</v>
+        <v>-1.0444444444444445</v>
       </c>
       <c r="H11" s="1">
         <v>-1</v>
@@ -3600,7 +3663,7 @@
       </c>
       <c r="B12" s="1">
         <f>(G12*-A7)+A8</f>
-        <v>1.48</v>
+        <v>1.5499999999999998</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
@@ -3608,7 +3671,7 @@
       </c>
       <c r="G12" s="1">
         <f>F12/G7</f>
-        <v>-0.9</v>
+        <v>-1</v>
       </c>
       <c r="H12" s="1">
         <v>-1</v>
@@ -3623,7 +3686,7 @@
       </c>
       <c r="B13" s="1">
         <f>(G13*-A7)+A8</f>
-        <v>1.452</v>
+        <v>1.5188888888888887</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
@@ -3631,7 +3694,7 @@
       </c>
       <c r="G13" s="1">
         <f>F13/G7</f>
-        <v>-0.86</v>
+        <v>-0.9555555555555556</v>
       </c>
       <c r="H13" s="1">
         <v>-1</v>
@@ -3646,7 +3709,7 @@
       </c>
       <c r="B14" s="1">
         <f>(G14*-A7)+A8</f>
-        <v>1.4239999999999999</v>
+        <v>1.4877777777777776</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
@@ -3654,7 +3717,7 @@
       </c>
       <c r="G14" s="1">
         <f>F14/G7</f>
-        <v>-0.82</v>
+        <v>-0.91111111111111109</v>
       </c>
       <c r="H14" s="1">
         <v>-1</v>
@@ -3669,7 +3732,7 @@
       </c>
       <c r="B15" s="1">
         <f>(G15*-A7)+A8</f>
-        <v>1.3959999999999999</v>
+        <v>1.4566666666666666</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
@@ -3677,14 +3740,10 @@
       </c>
       <c r="G15" s="1">
         <f>F15/G7</f>
-        <v>-0.78</v>
+        <v>-0.8666666666666667</v>
       </c>
       <c r="H15" s="1">
         <v>-1</v>
-      </c>
-      <c r="I15" s="1">
-        <f>(F15/40)^3</f>
-        <v>-0.92685937499999993</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3693,7 +3752,7 @@
       </c>
       <c r="B16" s="1">
         <f>(G16*-A7)+A8</f>
-        <v>1.3679999999999999</v>
+        <v>1.4255555555555555</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
@@ -3701,14 +3760,10 @@
       </c>
       <c r="G16" s="1">
         <f>F16/G7</f>
-        <v>-0.74</v>
+        <v>-0.82222222222222219</v>
       </c>
       <c r="H16" s="1">
         <v>-1</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" ref="I16:I55" si="1">(F16/40)^3</f>
-        <v>-0.79145312500000009</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3717,7 +3772,7 @@
       </c>
       <c r="B17" s="1">
         <f>(G17*-A7)+A8</f>
-        <v>1.3399999999999999</v>
+        <v>1.3944444444444444</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
@@ -3725,15 +3780,11 @@
       </c>
       <c r="G17" s="1">
         <f>F17/G7</f>
-        <v>-0.7</v>
+        <v>-0.77777777777777779</v>
       </c>
       <c r="H17" s="1">
-        <f>-1*(F17/35)^2</f>
+        <f t="shared" ref="H17:H34" si="1">-1*(F17/35)^2</f>
         <v>-1</v>
-      </c>
-      <c r="I17" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.669921875</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3742,7 +3793,7 @@
       </c>
       <c r="B18" s="1">
         <f>(G18*-A7)+A8</f>
-        <v>1.3119999999999998</v>
+        <v>1.3633333333333333</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
@@ -3750,15 +3801,15 @@
       </c>
       <c r="G18" s="1">
         <f>F18/G7</f>
-        <v>-0.66</v>
+        <v>-0.73333333333333328</v>
       </c>
       <c r="H18" s="1">
-        <f>-1*(F18/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.88897959183673469</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.56151562499999996</v>
+        <f>(F18/I7)^3</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3767,7 +3818,7 @@
       </c>
       <c r="B19" s="1">
         <f>(G19*-A7)+A8</f>
-        <v>1.284</v>
+        <v>1.3322222222222222</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
@@ -3775,15 +3826,15 @@
       </c>
       <c r="G19" s="1">
         <f>F19/G7</f>
-        <v>-0.62</v>
+        <v>-0.68888888888888888</v>
       </c>
       <c r="H19" s="1">
-        <f>-1*(F19/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.78448979591836732</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.46548437500000006</v>
+        <f>(F19/I7)^3</f>
+        <v>-0.82897849013551506</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3792,7 +3843,7 @@
       </c>
       <c r="B20" s="1">
         <f>(G20*-A7)+A8</f>
-        <v>1.256</v>
+        <v>1.3011111111111111</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
@@ -3800,15 +3851,15 @@
       </c>
       <c r="G20" s="1">
         <f>F20/G7</f>
-        <v>-0.57999999999999996</v>
+        <v>-0.64444444444444449</v>
       </c>
       <c r="H20" s="1">
-        <f>-1*(F20/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.68653061224489809</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.38107812499999999</v>
+        <f>(F20/I7)^3</f>
+        <v>-0.67865987700698438</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3817,7 +3868,7 @@
       </c>
       <c r="B21" s="1">
         <f>(G21*-A7)+A8</f>
-        <v>1.228</v>
+        <v>1.27</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
@@ -3825,15 +3876,15 @@
       </c>
       <c r="G21" s="1">
         <f>F21/G7</f>
-        <v>-0.54</v>
+        <v>-0.6</v>
       </c>
       <c r="H21" s="1">
-        <f>-1*(F21/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.59510204081632656</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.30754687500000005</v>
+        <f>(F21/I7)^3</f>
+        <v>-0.54770848985725029</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3842,7 +3893,7 @@
       </c>
       <c r="B22" s="1">
         <f>(G22*-A7)+A8</f>
-        <v>1.2</v>
+        <v>1.2388888888888889</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
@@ -3850,15 +3901,15 @@
       </c>
       <c r="G22" s="1">
         <f>F22/G7</f>
-        <v>-0.5</v>
+        <v>-0.55555555555555558</v>
       </c>
       <c r="H22" s="1">
-        <f>-1*(F22/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.51020408163265307</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.244140625</v>
+        <f>(F22/I7)^3</f>
+        <v>-0.43478865792915378</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3867,7 +3918,7 @@
       </c>
       <c r="B23" s="1">
         <f>(G23*-A7)+A8</f>
-        <v>1.1719999999999999</v>
+        <v>1.2077777777777778</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
@@ -3875,15 +3926,15 @@
       </c>
       <c r="G23" s="1">
         <f>F23/G7</f>
-        <v>-0.46</v>
+        <v>-0.51111111111111107</v>
       </c>
       <c r="H23" s="1">
-        <f>-1*(F23/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.43183673469387757</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.19010937499999994</v>
+        <f>(F23/I7)^3</f>
+        <v>-0.33856471046553699</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3892,7 +3943,7 @@
       </c>
       <c r="B24" s="1">
         <f>(G24*-A7)+A8</f>
-        <v>1.1439999999999999</v>
+        <v>1.1766666666666667</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
@@ -3900,15 +3951,15 @@
       </c>
       <c r="G24" s="1">
         <f>F24/G7</f>
-        <v>-0.42</v>
+        <v>-0.46666666666666667</v>
       </c>
       <c r="H24" s="1">
-        <f>-1*(F24/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.36</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.14470312500000002</v>
+        <f>(F24/I7)^3</f>
+        <v>-0.25770097670924114</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3917,7 +3968,7 @@
       </c>
       <c r="B25" s="1">
         <f>(G25*-A7)+A8</f>
-        <v>1.1159999999999999</v>
+        <v>1.1455555555555554</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
@@ -3925,15 +3976,15 @@
       </c>
       <c r="G25" s="1">
         <f>F25/G7</f>
-        <v>-0.38</v>
+        <v>-0.42222222222222222</v>
       </c>
       <c r="H25" s="1">
-        <f>-1*(F25/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.29469387755102039</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.10717187499999999</v>
+        <f>(F25/I7)^3</f>
+        <v>-0.19086178590310826</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3942,7 +3993,7 @@
       </c>
       <c r="B26" s="1">
         <f>(G26*-A7)+A8</f>
-        <v>1.0880000000000001</v>
+        <v>1.1144444444444443</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
@@ -3950,15 +4001,15 @@
       </c>
       <c r="G26" s="1">
         <f>F26/G7</f>
-        <v>-0.34</v>
+        <v>-0.37777777777777777</v>
       </c>
       <c r="H26" s="1">
-        <f>-1*(F26/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.23591836734693877</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="1"/>
-        <v>-7.676562499999999E-2</v>
+        <f>(F26/I7)^3</f>
+        <v>-0.13671146728997968</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3967,7 +4018,7 @@
       </c>
       <c r="B27" s="1">
         <f>(G27*-A7)+A8</f>
-        <v>1.06</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
@@ -3975,15 +4026,15 @@
       </c>
       <c r="G27" s="1">
         <f>F27/G7</f>
-        <v>-0.3</v>
+        <v>-0.33333333333333331</v>
       </c>
       <c r="H27" s="1">
-        <f>-1*(F27/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.18367346938775508</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="1"/>
-        <v>-5.2734375E-2</v>
+        <f>(F27/I7)^3</f>
+        <v>-9.3914350112697206E-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3992,7 +4043,7 @@
       </c>
       <c r="B28" s="1">
         <f>(G28*-A7)+A8</f>
-        <v>1.032</v>
+        <v>1.0522222222222222</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
@@ -4000,15 +4051,15 @@
       </c>
       <c r="G28" s="1">
         <f>F28/G7</f>
-        <v>-0.26</v>
+        <v>-0.28888888888888886</v>
       </c>
       <c r="H28" s="1">
-        <f>-1*(F28/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-0.1379591836734694</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.4328125000000008E-2</v>
+        <f>(F28/I7)^3</f>
+        <v>-6.1134763614102451E-2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -4017,7 +4068,7 @@
       </c>
       <c r="B29" s="1">
         <f>(G29*-A7)+A8</f>
-        <v>1.004</v>
+        <v>1.0211111111111111</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
@@ -4025,15 +4076,15 @@
       </c>
       <c r="G29" s="1">
         <f>F29/G7</f>
-        <v>-0.22</v>
+        <v>-0.24444444444444444</v>
       </c>
       <c r="H29" s="1">
-        <f>-1*(F29/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-9.8775510204081624E-2</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.0796875000000006E-2</v>
+        <f>(F29/I7)^3</f>
+        <v>-3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4042,7 +4093,7 @@
       </c>
       <c r="B30" s="1">
         <f>(G30*-A7)+A8</f>
-        <v>0.97599999999999998</v>
+        <v>0.99</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
@@ -4050,15 +4101,15 @@
       </c>
       <c r="G30" s="1">
         <f>F30/G7</f>
-        <v>-0.18</v>
+        <v>-0.2</v>
       </c>
       <c r="H30" s="1">
-        <f>-1*(F30/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-6.6122448979591825E-2</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.1390625000000001E-2</v>
+        <f>(F30/I7)^3</f>
+        <v>-2.0285499624342593E-2</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4067,7 +4118,7 @@
       </c>
       <c r="B31" s="1">
         <f>(G31*-A7)+A8</f>
-        <v>0.94799999999999995</v>
+        <v>0.9588888888888889</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
@@ -4075,15 +4126,15 @@
       </c>
       <c r="G31" s="1">
         <f>F31/G7</f>
-        <v>-0.14000000000000001</v>
+        <v>-0.15555555555555556</v>
       </c>
       <c r="H31" s="1">
-        <f>-1*(F31/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-4.0000000000000008E-2</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="1"/>
-        <v>-5.3593749999999987E-3</v>
+        <f>(F31/I7)^3</f>
+        <v>-9.5444806188607848E-3</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4092,7 +4143,7 @@
       </c>
       <c r="B32" s="1">
         <f>(G32*-A7)+A8</f>
-        <v>0.91999999999999993</v>
+        <v>0.9277777777777777</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
@@ -4100,15 +4151,15 @@
       </c>
       <c r="G32" s="1">
         <f>F32/G7</f>
-        <v>-0.1</v>
+        <v>-0.1111111111111111</v>
       </c>
       <c r="H32" s="1">
-        <f>-1*(F32/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-2.0408163265306121E-2</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.953125E-3</v>
+        <f>(F32/I7)^3</f>
+        <v>-3.4783092634332307E-3</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -4117,7 +4168,7 @@
       </c>
       <c r="B33" s="1">
         <f>(G33*-A7)+A8</f>
-        <v>0.89200000000000002</v>
+        <v>0.89666666666666661</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="0"/>
@@ -4125,15 +4176,15 @@
       </c>
       <c r="G33" s="1">
         <f>F33/G7</f>
-        <v>-0.06</v>
+        <v>-6.6666666666666666E-2</v>
       </c>
       <c r="H33" s="1">
-        <f>-1*(F33/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-7.3469387755102046E-3</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="1"/>
-        <v>-4.21875E-4</v>
+        <f>(F33/I7)^3</f>
+        <v>-7.513148009015778E-4</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4142,7 +4193,7 @@
       </c>
       <c r="B34" s="1">
         <f>(G34*-A7)+A8</f>
-        <v>0.86399999999999999</v>
+        <v>0.86555555555555552</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="0"/>
@@ -4150,15 +4201,15 @@
       </c>
       <c r="G34" s="1">
         <f>F34/G7</f>
-        <v>-0.02</v>
+        <v>-2.2222222222222223E-2</v>
       </c>
       <c r="H34" s="1">
-        <f>-1*(F34/35)^2</f>
+        <f t="shared" si="1"/>
         <v>-8.1632653061224482E-4</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.5625000000000004E-5</v>
+        <f>(F34/I7)^3</f>
+        <v>-2.7826474107465846E-5</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4178,11 +4229,11 @@
         <v>0</v>
       </c>
       <c r="H35" s="1">
-        <f t="shared" ref="H18:H52" si="2">(F35/35)^2</f>
+        <f t="shared" ref="H35:H52" si="2">(F35/35)^2</f>
         <v>0</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="1"/>
+        <f>(F35/I7)^3</f>
         <v>0</v>
       </c>
     </row>
@@ -4192,7 +4243,7 @@
       </c>
       <c r="B36" s="1">
         <f>(G36*-A7)+A8</f>
-        <v>0.83599999999999997</v>
+        <v>0.83444444444444443</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="0"/>
@@ -4200,15 +4251,15 @@
       </c>
       <c r="G36" s="1">
         <f>F36/G7</f>
-        <v>0.02</v>
+        <v>2.2222222222222223E-2</v>
       </c>
       <c r="H36" s="1">
         <f t="shared" si="2"/>
         <v>8.1632653061224482E-4</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="1"/>
-        <v>1.5625000000000004E-5</v>
+        <f>(F36/I7)^3</f>
+        <v>2.7826474107465846E-5</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4217,7 +4268,7 @@
       </c>
       <c r="B37" s="1">
         <f>(G37*-A7)+A8</f>
-        <v>0.80799999999999994</v>
+        <v>0.80333333333333334</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="0"/>
@@ -4225,15 +4276,15 @@
       </c>
       <c r="G37" s="1">
         <f>F37/G7</f>
-        <v>0.06</v>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="H37" s="1">
         <f t="shared" si="2"/>
         <v>7.3469387755102046E-3</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="1"/>
-        <v>4.21875E-4</v>
+        <f>(F37/I7)^3</f>
+        <v>7.513148009015778E-4</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4242,7 +4293,7 @@
       </c>
       <c r="B38" s="1">
         <f>(G38*-A7)+A8</f>
-        <v>0.78</v>
+        <v>0.77222222222222225</v>
       </c>
       <c r="F38" s="1">
         <f t="shared" si="0"/>
@@ -4250,15 +4301,15 @@
       </c>
       <c r="G38" s="1">
         <f>F38/G7</f>
-        <v>0.1</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H38" s="1">
         <f t="shared" si="2"/>
         <v>2.0408163265306121E-2</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="1"/>
-        <v>1.953125E-3</v>
+        <f>(F38/I7)^3</f>
+        <v>3.4783092634332307E-3</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4267,7 +4318,7 @@
       </c>
       <c r="B39" s="1">
         <f>(G39*-A7)+A8</f>
-        <v>0.752</v>
+        <v>0.74111111111111105</v>
       </c>
       <c r="F39" s="1">
         <f t="shared" si="0"/>
@@ -4275,14 +4326,14 @@
       </c>
       <c r="G39" s="1">
         <f>F39/G7</f>
-        <v>0.14000000000000001</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="H39" s="1">
         <f t="shared" si="2"/>
         <v>4.0000000000000008E-2</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="1"/>
+        <f>(F39/40)^3</f>
         <v>5.3593749999999987E-3</v>
       </c>
     </row>
@@ -4292,7 +4343,7 @@
       </c>
       <c r="B40" s="1">
         <f>(G40*-A7)+A8</f>
-        <v>0.72399999999999998</v>
+        <v>0.71</v>
       </c>
       <c r="F40" s="1">
         <f t="shared" si="0"/>
@@ -4300,15 +4351,15 @@
       </c>
       <c r="G40" s="1">
         <f>F40/G7</f>
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="H40" s="1">
         <f t="shared" si="2"/>
         <v>6.6122448979591825E-2</v>
       </c>
-      <c r="I40" s="1">
-        <f t="shared" si="1"/>
-        <v>1.1390625000000001E-2</v>
+      <c r="I40" s="5">
+        <f>(F40/I7)^3</f>
+        <v>2.0285499624342593E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4317,7 +4368,7 @@
       </c>
       <c r="B41" s="1">
         <f>(G41*-A7)+A8</f>
-        <v>0.69599999999999995</v>
+        <v>0.67888888888888888</v>
       </c>
       <c r="F41" s="1">
         <f t="shared" si="0"/>
@@ -4325,15 +4376,15 @@
       </c>
       <c r="G41" s="1">
         <f>F41/G7</f>
-        <v>0.22</v>
+        <v>0.24444444444444444</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" si="2"/>
         <v>9.8775510204081624E-2</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="1"/>
-        <v>2.0796875000000006E-2</v>
+        <f>(F41/I7)^3</f>
+        <v>3.7037037037037035E-2</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4342,7 +4393,7 @@
       </c>
       <c r="B42" s="1">
         <f>(G42*-A7)+A8</f>
-        <v>0.66799999999999993</v>
+        <v>0.64777777777777779</v>
       </c>
       <c r="F42" s="1">
         <f t="shared" si="0"/>
@@ -4350,15 +4401,15 @@
       </c>
       <c r="G42" s="1">
         <f>F42/G7</f>
-        <v>0.26</v>
+        <v>0.28888888888888886</v>
       </c>
       <c r="H42" s="1">
         <f t="shared" si="2"/>
         <v>0.1379591836734694</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="1"/>
-        <v>3.4328125000000008E-2</v>
+        <f>(F42/I7)^3</f>
+        <v>6.1134763614102451E-2</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4367,7 +4418,7 @@
       </c>
       <c r="B43" s="1">
         <f>(G43*-A7)+A8</f>
-        <v>0.64</v>
+        <v>0.6166666666666667</v>
       </c>
       <c r="F43" s="1">
         <f t="shared" si="0"/>
@@ -4375,15 +4426,15 @@
       </c>
       <c r="G43" s="1">
         <f>F43/G7</f>
-        <v>0.3</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" si="2"/>
         <v>0.18367346938775508</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" si="1"/>
-        <v>5.2734375E-2</v>
+        <f>(F43/I7)^3</f>
+        <v>9.3914350112697206E-2</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4392,7 +4443,7 @@
       </c>
       <c r="B44" s="1">
         <f>(G44*-A7)+A8</f>
-        <v>0.61199999999999999</v>
+        <v>0.58555555555555561</v>
       </c>
       <c r="F44" s="1">
         <f t="shared" si="0"/>
@@ -4400,15 +4451,15 @@
       </c>
       <c r="G44" s="1">
         <f>F44/G7</f>
-        <v>0.34</v>
+        <v>0.37777777777777777</v>
       </c>
       <c r="H44" s="1">
         <f t="shared" si="2"/>
         <v>0.23591836734693877</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" si="1"/>
-        <v>7.676562499999999E-2</v>
+        <f>(F44/I7)^3</f>
+        <v>0.13671146728997968</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -4417,7 +4468,7 @@
       </c>
       <c r="B45" s="1">
         <f>(G45*-A7)+A8</f>
-        <v>0.58400000000000007</v>
+        <v>0.55444444444444452</v>
       </c>
       <c r="F45" s="1">
         <f t="shared" si="0"/>
@@ -4425,15 +4476,15 @@
       </c>
       <c r="G45" s="1">
         <f>F45/G7</f>
-        <v>0.38</v>
+        <v>0.42222222222222222</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" si="2"/>
         <v>0.29469387755102039</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="1"/>
-        <v>0.10717187499999999</v>
+        <f>(F45/I7)^3</f>
+        <v>0.19086178590310826</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -4442,7 +4493,7 @@
       </c>
       <c r="B46" s="1">
         <f>(G46*-A7)+A8</f>
-        <v>0.55600000000000005</v>
+        <v>0.52333333333333332</v>
       </c>
       <c r="F46" s="1">
         <f t="shared" si="0"/>
@@ -4450,15 +4501,15 @@
       </c>
       <c r="G46" s="1">
         <f>F46/G7</f>
-        <v>0.42</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="H46" s="1">
         <f t="shared" si="2"/>
         <v>0.36</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" si="1"/>
-        <v>0.14470312500000002</v>
+        <f>(F46/I7)^3</f>
+        <v>0.25770097670924114</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4467,7 +4518,7 @@
       </c>
       <c r="B47" s="1">
         <f>(G47*-A7)+A8</f>
-        <v>0.52800000000000002</v>
+        <v>0.49222222222222223</v>
       </c>
       <c r="F47" s="1">
         <f t="shared" si="0"/>
@@ -4475,15 +4526,15 @@
       </c>
       <c r="G47" s="1">
         <f>F47/G7</f>
-        <v>0.46</v>
+        <v>0.51111111111111107</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="2"/>
         <v>0.43183673469387757</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="1"/>
-        <v>0.19010937499999994</v>
+        <f>(F47/I7)^3</f>
+        <v>0.33856471046553699</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4492,7 +4543,7 @@
       </c>
       <c r="B48" s="1">
         <f>(G48*-A7)+A8</f>
-        <v>0.5</v>
+        <v>0.46111111111111108</v>
       </c>
       <c r="F48" s="1">
         <f t="shared" si="0"/>
@@ -4500,15 +4551,15 @@
       </c>
       <c r="G48" s="1">
         <f>F48/G7</f>
-        <v>0.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="H48" s="1">
         <f t="shared" si="2"/>
         <v>0.51020408163265307</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="1"/>
-        <v>0.244140625</v>
+        <f>(F48/I7)^3</f>
+        <v>0.43478865792915378</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4517,7 +4568,7 @@
       </c>
       <c r="B49" s="1">
         <f>(G49*-A7)+A8</f>
-        <v>0.47199999999999998</v>
+        <v>0.43</v>
       </c>
       <c r="F49" s="1">
         <f t="shared" si="0"/>
@@ -4525,15 +4576,15 @@
       </c>
       <c r="G49" s="1">
         <f>F49/G7</f>
-        <v>0.54</v>
+        <v>0.6</v>
       </c>
       <c r="H49" s="1">
         <f t="shared" si="2"/>
         <v>0.59510204081632656</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="1"/>
-        <v>0.30754687500000005</v>
+        <f>(F49/I7)^3</f>
+        <v>0.54770848985725029</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4542,7 +4593,7 @@
       </c>
       <c r="B50" s="1">
         <f>(G50*-A7)+A8</f>
-        <v>0.44400000000000001</v>
+        <v>0.39888888888888885</v>
       </c>
       <c r="F50" s="1">
         <f t="shared" si="0"/>
@@ -4550,15 +4601,15 @@
       </c>
       <c r="G50" s="1">
         <f>F50/G7</f>
-        <v>0.57999999999999996</v>
+        <v>0.64444444444444449</v>
       </c>
       <c r="H50" s="1">
         <f t="shared" si="2"/>
         <v>0.68653061224489809</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="1"/>
-        <v>0.38107812499999999</v>
+        <f>(F50/I7)^3</f>
+        <v>0.67865987700698438</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4567,7 +4618,7 @@
       </c>
       <c r="B51" s="1">
         <f>(G51*-A7)+A8</f>
-        <v>0.41599999999999998</v>
+        <v>0.36777777777777781</v>
       </c>
       <c r="F51" s="1">
         <f t="shared" si="0"/>
@@ -4575,15 +4626,15 @@
       </c>
       <c r="G51" s="1">
         <f>F51/G7</f>
-        <v>0.62</v>
+        <v>0.68888888888888888</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" si="2"/>
         <v>0.78448979591836732</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="1"/>
-        <v>0.46548437500000006</v>
+        <f>(F51/I7)^3</f>
+        <v>0.82897849013551506</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4592,7 +4643,7 @@
       </c>
       <c r="B52" s="1">
         <f>(G52*-A7)+A8</f>
-        <v>0.38800000000000001</v>
+        <v>0.33666666666666667</v>
       </c>
       <c r="F52" s="1">
         <f t="shared" si="0"/>
@@ -4600,15 +4651,15 @@
       </c>
       <c r="G52" s="1">
         <f>F52/G7</f>
-        <v>0.66</v>
+        <v>0.73333333333333328</v>
       </c>
       <c r="H52" s="1">
         <f t="shared" si="2"/>
         <v>0.88897959183673469</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="1"/>
-        <v>0.56151562499999996</v>
+        <f>(F52/I7)^3</f>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4617,7 +4668,7 @@
       </c>
       <c r="B53" s="1">
         <f>(G53*-A7)+A8</f>
-        <v>0.36000000000000004</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="F53" s="1">
         <f t="shared" si="0"/>
@@ -4625,15 +4676,11 @@
       </c>
       <c r="G53" s="1">
         <f>F53/G7</f>
-        <v>0.7</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" ref="H36:H53" si="3">(F53/35)*(F53/35)</f>
+        <f t="shared" ref="H53" si="3">(F53/35)*(F53/35)</f>
         <v>1</v>
-      </c>
-      <c r="I53" s="1">
-        <f t="shared" si="1"/>
-        <v>0.669921875</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4642,7 +4689,7 @@
       </c>
       <c r="B54" s="1">
         <f>(G54*-A7)+A8</f>
-        <v>0.33199999999999996</v>
+        <v>0.27444444444444449</v>
       </c>
       <c r="F54" s="1">
         <f t="shared" si="0"/>
@@ -4650,14 +4697,10 @@
       </c>
       <c r="G54" s="1">
         <f>F54/G7</f>
-        <v>0.74</v>
+        <v>0.82222222222222219</v>
       </c>
       <c r="H54" s="1">
         <v>1</v>
-      </c>
-      <c r="I54" s="1">
-        <f t="shared" si="1"/>
-        <v>0.79145312500000009</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -4666,7 +4709,7 @@
       </c>
       <c r="B55" s="1">
         <f>(G55*-A7)+A8</f>
-        <v>0.30400000000000005</v>
+        <v>0.24333333333333329</v>
       </c>
       <c r="F55" s="1">
         <f t="shared" si="0"/>
@@ -4674,14 +4717,10 @@
       </c>
       <c r="G55" s="1">
         <f>F55/G7</f>
-        <v>0.78</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="H55" s="1">
         <v>1</v>
-      </c>
-      <c r="I55" s="1">
-        <f t="shared" si="1"/>
-        <v>0.92685937499999993</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4690,7 +4729,7 @@
       </c>
       <c r="B56" s="1">
         <f>(G56*-A7)+A8</f>
-        <v>0.27600000000000002</v>
+        <v>0.2122222222222222</v>
       </c>
       <c r="F56" s="1">
         <f t="shared" si="0"/>
@@ -4698,7 +4737,7 @@
       </c>
       <c r="G56" s="1">
         <f>F56/G7</f>
-        <v>0.82</v>
+        <v>0.91111111111111109</v>
       </c>
       <c r="H56" s="1">
         <v>1</v>
@@ -4713,7 +4752,7 @@
       </c>
       <c r="B57" s="1">
         <f>(G57*-A7)+A8</f>
-        <v>0.248</v>
+        <v>0.18111111111111111</v>
       </c>
       <c r="F57" s="1">
         <f t="shared" si="0"/>
@@ -4721,7 +4760,7 @@
       </c>
       <c r="G57" s="1">
         <f>F57/G7</f>
-        <v>0.86</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="H57" s="1">
         <v>1</v>
@@ -4736,7 +4775,7 @@
       </c>
       <c r="B58" s="1">
         <f>(G58*-A7)+A8</f>
-        <v>0.21999999999999997</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="F58" s="1">
         <f t="shared" si="0"/>
@@ -4744,7 +4783,7 @@
       </c>
       <c r="G58" s="1">
         <f>F58/G7</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="H58" s="1">
         <v>1</v>
@@ -4759,7 +4798,7 @@
       </c>
       <c r="B59" s="1">
         <f>(G59*-A7)+A8</f>
-        <v>0.19200000000000006</v>
+        <v>0.11888888888888882</v>
       </c>
       <c r="F59" s="1">
         <f t="shared" si="0"/>
@@ -4767,7 +4806,7 @@
       </c>
       <c r="G59" s="1">
         <f>F59/G7</f>
-        <v>0.94</v>
+        <v>1.0444444444444445</v>
       </c>
       <c r="H59" s="1">
         <v>1</v>
@@ -4782,7 +4821,7 @@
       </c>
       <c r="B60" s="1">
         <f>(G60*-A7)+A8</f>
-        <v>0.16400000000000003</v>
+        <v>8.7777777777777843E-2</v>
       </c>
       <c r="F60" s="1">
         <f t="shared" si="0"/>
@@ -4790,7 +4829,7 @@
       </c>
       <c r="G60" s="1">
         <f>F60/G7</f>
-        <v>0.98</v>
+        <v>1.0888888888888888</v>
       </c>
       <c r="H60" s="1">
         <v>1</v>
@@ -4807,4 +4846,300 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:I19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="6" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>0.4</v>
+      </c>
+      <c r="F5">
+        <v>0.3</v>
+      </c>
+      <c r="G5">
+        <v>5.95</v>
+      </c>
+      <c r="H5">
+        <v>5.87</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6">
+        <v>0.4</v>
+      </c>
+      <c r="F6">
+        <v>0.3</v>
+      </c>
+      <c r="G6">
+        <v>5.37</v>
+      </c>
+      <c r="H6">
+        <v>5.42</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7">
+        <v>0.4</v>
+      </c>
+      <c r="F7">
+        <v>0.3</v>
+      </c>
+      <c r="G7">
+        <v>5.61</v>
+      </c>
+      <c r="H7">
+        <v>5.5</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8">
+        <v>0.4</v>
+      </c>
+      <c r="F8">
+        <v>0.3</v>
+      </c>
+      <c r="G8">
+        <v>5.66</v>
+      </c>
+      <c r="H8">
+        <v>5.65</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>0.4</v>
+      </c>
+      <c r="F10">
+        <v>0.3</v>
+      </c>
+      <c r="G10">
+        <v>5.89</v>
+      </c>
+      <c r="H10">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="9"/>
+      <c r="E11">
+        <v>0.4</v>
+      </c>
+      <c r="F11">
+        <v>0.3</v>
+      </c>
+      <c r="G11">
+        <v>5.33</v>
+      </c>
+      <c r="H11">
+        <v>5.39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="9"/>
+      <c r="E12">
+        <v>0.4</v>
+      </c>
+      <c r="F12">
+        <v>0.3</v>
+      </c>
+      <c r="G12">
+        <v>5.66</v>
+      </c>
+      <c r="H12">
+        <v>5.58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="9"/>
+      <c r="E13">
+        <v>0.4</v>
+      </c>
+      <c r="F13">
+        <v>0.3</v>
+      </c>
+      <c r="G13">
+        <v>5.71</v>
+      </c>
+      <c r="H13">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>5.53</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>5.54</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>5.63</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D10:D13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final project updated Algorithms of Oscar added
</commit_message>
<xml_diff>
--- a/FreescaleCup2013/testing/Algorithm_ORA/Algorithms.xlsx
+++ b/FreescaleCup2013/testing/Algorithm_ORA/Algorithms.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Speed</t>
   </si>
@@ -113,6 +113,9 @@
   <si>
     <t>diff/45</t>
   </si>
+  <si>
+    <t>diff/70</t>
+  </si>
 </sst>
 </file>
 
@@ -170,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -183,6 +186,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,6 +240,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-MX"/>
+              <a:t>Steering</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -458,7 +492,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>NoDummy!$G$10:$G$60</c:f>
+              <c:f>NoDummy!$H$10:$H$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -811,7 +845,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>NoDummy!$H$10:$H$60</c:f>
+              <c:f>NoDummy!$I$10:$I$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1170,7 +1204,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>NoDummy!$I$10:$I$60</c:f>
+              <c:f>NoDummy!$J$10:$J$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -1322,8 +1356,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="183750384"/>
-        <c:axId val="183750944"/>
+        <c:axId val="184479520"/>
+        <c:axId val="184480080"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1534,158 +1568,128 @@
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="51"/>
-                      <c:pt idx="0">
-                        <c:v>1.612222222222222</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>1.5811111111111111</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>1.5499999999999998</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>1.5188888888888887</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>1.4877777777777776</c:v>
-                      </c:pt>
                       <c:pt idx="5">
-                        <c:v>1.4566666666666666</c:v>
+                        <c:v>-0.11428571428571432</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>1.4255555555555555</c:v>
+                        <c:v>-5.7142857142857162E-2</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>1.3944444444444444</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>1.3633333333333333</c:v>
+                        <c:v>5.7142857142857162E-2</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>1.3322222222222222</c:v>
+                        <c:v>0.11428571428571432</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>1.3011111111111111</c:v>
+                        <c:v>0.17142857142857137</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>1.27</c:v>
+                        <c:v>0.22857142857142854</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>1.2388888888888889</c:v>
+                        <c:v>0.2857142857142857</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>1.2077777777777778</c:v>
+                        <c:v>0.34285714285714286</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>1.1766666666666667</c:v>
+                        <c:v>0.4</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>1.1455555555555554</c:v>
+                        <c:v>0.45714285714285718</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>1.1144444444444443</c:v>
+                        <c:v>0.51428571428571423</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>1.0833333333333333</c:v>
+                        <c:v>0.5714285714285714</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>1.0522222222222222</c:v>
+                        <c:v>0.62857142857142856</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>1.0211111111111111</c:v>
+                        <c:v>0.68571428571428572</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>0.99</c:v>
+                        <c:v>0.74285714285714288</c:v>
                       </c:pt>
                       <c:pt idx="21">
-                        <c:v>0.9588888888888889</c:v>
+                        <c:v>0.8</c:v>
                       </c:pt>
                       <c:pt idx="22">
-                        <c:v>0.9277777777777777</c:v>
+                        <c:v>0.85714285714285721</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>0.89666666666666661</c:v>
+                        <c:v>0.91428571428571426</c:v>
                       </c:pt>
                       <c:pt idx="24">
-                        <c:v>0.86555555555555552</c:v>
+                        <c:v>0.97142857142857142</c:v>
                       </c:pt>
                       <c:pt idx="25">
-                        <c:v>0.85</c:v>
+                        <c:v>1</c:v>
                       </c:pt>
                       <c:pt idx="26">
-                        <c:v>0.83444444444444443</c:v>
+                        <c:v>0.97142857142857142</c:v>
                       </c:pt>
                       <c:pt idx="27">
-                        <c:v>0.80333333333333334</c:v>
+                        <c:v>0.91428571428571426</c:v>
                       </c:pt>
                       <c:pt idx="28">
-                        <c:v>0.77222222222222225</c:v>
+                        <c:v>0.85714285714285721</c:v>
                       </c:pt>
                       <c:pt idx="29">
-                        <c:v>0.74111111111111105</c:v>
+                        <c:v>0.8</c:v>
                       </c:pt>
                       <c:pt idx="30">
-                        <c:v>0.71</c:v>
+                        <c:v>0.74285714285714288</c:v>
                       </c:pt>
                       <c:pt idx="31">
-                        <c:v>0.67888888888888888</c:v>
+                        <c:v>0.68571428571428572</c:v>
                       </c:pt>
                       <c:pt idx="32">
-                        <c:v>0.64777777777777779</c:v>
+                        <c:v>0.62857142857142856</c:v>
                       </c:pt>
                       <c:pt idx="33">
-                        <c:v>0.6166666666666667</c:v>
+                        <c:v>0.5714285714285714</c:v>
                       </c:pt>
                       <c:pt idx="34">
-                        <c:v>0.58555555555555561</c:v>
+                        <c:v>0.51428571428571423</c:v>
                       </c:pt>
                       <c:pt idx="35">
-                        <c:v>0.55444444444444452</c:v>
+                        <c:v>0.45714285714285718</c:v>
                       </c:pt>
                       <c:pt idx="36">
-                        <c:v>0.52333333333333332</c:v>
+                        <c:v>0.4</c:v>
                       </c:pt>
                       <c:pt idx="37">
-                        <c:v>0.49222222222222223</c:v>
+                        <c:v>0.34285714285714286</c:v>
                       </c:pt>
                       <c:pt idx="38">
-                        <c:v>0.46111111111111108</c:v>
+                        <c:v>0.2857142857142857</c:v>
                       </c:pt>
                       <c:pt idx="39">
-                        <c:v>0.43</c:v>
+                        <c:v>0.22857142857142854</c:v>
                       </c:pt>
                       <c:pt idx="40">
-                        <c:v>0.39888888888888885</c:v>
+                        <c:v>0.17142857142857137</c:v>
                       </c:pt>
                       <c:pt idx="41">
-                        <c:v>0.36777777777777781</c:v>
+                        <c:v>0.11428571428571432</c:v>
                       </c:pt>
                       <c:pt idx="42">
-                        <c:v>0.33666666666666667</c:v>
+                        <c:v>5.7142857142857162E-2</c:v>
                       </c:pt>
                       <c:pt idx="43">
-                        <c:v>0.30555555555555558</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="44">
-                        <c:v>0.27444444444444449</c:v>
+                        <c:v>-5.7142857142857162E-2</c:v>
                       </c:pt>
                       <c:pt idx="45">
-                        <c:v>0.24333333333333329</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>0.2122222222222222</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>0.18111111111111111</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>0.15000000000000002</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>0.11888888888888882</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>8.7777777777777843E-2</c:v>
+                        <c:v>-0.11428571428571432</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -1901,6 +1905,99 @@
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="51"/>
+                      <c:pt idx="10">
+                        <c:v>0.31346938775510191</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.40489795918367344</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.48979591836734693</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.56816326530612238</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.64</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.70530612244897961</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.76408163265306128</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.81632653061224492</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.86204081632653062</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.9012244897959184</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.93387755102040815</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.96</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.97959183673469385</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.99265306122448982</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.99918367346938775</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.99918367346938775</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>0.99265306122448982</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>0.97959183673469385</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>0.96</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0.93387755102040815</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0.9012244897959184</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0.86204081632653062</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0.81632653061224492</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0.76408163265306128</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0.70530612244897961</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0.64</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0.56816326530612238</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0.48979591836734693</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0.40489795918367344</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0.31346938775510191</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
@@ -2115,6 +2212,99 @@
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="51"/>
+                      <c:pt idx="10">
+                        <c:v>0.32134012299301562</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.45229151014274971</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.56521134207084622</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.66143528953446307</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.74229902329075892</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.80913821409689168</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.86328853271002037</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.90608564988730278</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.93886523638589758</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.96296296296296302</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.97971450037565744</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.99045551938113918</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.99652169073656682</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.99924868519909837</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.99997217352589252</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>1</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.99997217352589252</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>0.99924868519909837</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>0.99652169073656682</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>0.99045551938113918</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0.97971450037565744</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0.96296296296296302</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0.93886523638589758</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0.90608564988730278</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0.86328853271002037</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0.80913821409689168</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0.74229902329075892</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0.66143528953446307</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0.56521134207084622</c:v>
+                      </c:pt>
+                      <c:pt idx="39">
+                        <c:v>0.45229151014274971</c:v>
+                      </c:pt>
+                      <c:pt idx="40">
+                        <c:v>0.32134012299301562</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
@@ -2322,7 +2512,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>NoDummy!$F$10:$F$60</c15:sqref>
+                          <c15:sqref>NoDummy!$G$10:$G$60</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -2492,7 +2682,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="183750384"/>
+        <c:axId val="184479520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2549,12 +2739,12 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="183750944"/>
+        <c:crossAx val="184480080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183750944"/>
+        <c:axId val="184480080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,7 +2801,1147 @@
             <a:endParaRPr lang="es-MX"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="183750384"/>
+        <c:crossAx val="184479520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-MX"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-MX"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NoDummy!$A$10:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NoDummy!$B$10:$B$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="5">
+                  <c:v>-0.11428571428571432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.7142857142857162E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.7142857142857162E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11428571428571432</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.17142857142857137</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22857142857142854</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.34285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.45714285714285718</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.51428571428571423</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.62857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.68571428571428572</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.74285714285714288</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.85714285714285721</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.97142857142857142</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.97142857142857142</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.85714285714285721</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.74285714285714288</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.68571428571428572</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.62857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.51428571428571423</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.45714285714285718</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.34285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.22857142857142854</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.17142857142857137</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.11428571428571432</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.7142857142857162E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-5.7142857142857162E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.11428571428571432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NoDummy!$A$10:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NoDummy!$C$10:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="10">
+                  <c:v>0.31346938775510191</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.40489795918367344</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.48979591836734693</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56816326530612238</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.70530612244897961</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.76408163265306128</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.81632653061224492</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.86204081632653062</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9012244897959184</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.93387755102040815</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.97959183673469385</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99265306122448982</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99918367346938775</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99918367346938775</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99265306122448982</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.97959183673469385</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.93387755102040815</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.9012244897959184</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.86204081632653062</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.81632653061224492</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.76408163265306128</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.70530612244897961</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.56816326530612238</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.48979591836734693</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.40489795918367344</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.31346938775510191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>NoDummy!$A$10:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>112</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>NoDummy!$D$10:$D$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="10">
+                  <c:v>0.32134012299301562</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.45229151014274971</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.56521134207084622</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.66143528953446307</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.74229902329075892</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.80913821409689168</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.86328853271002037</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.90608564988730278</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.93886523638589758</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.96296296296296302</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.97971450037565744</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99045551938113918</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99652169073656682</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99924868519909837</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99997217352589252</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99997217352589252</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99924868519909837</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99652169073656682</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.99045551938113918</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.97971450037565744</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.96296296296296302</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.93886523638589758</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.90608564988730278</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.86328853271002037</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.80913821409689168</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.74229902329075892</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.66143528953446307</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.56521134207084622</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.45229151014274971</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.32134012299301562</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="251107920"/>
+        <c:axId val="255216640"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="251107920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="255216640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="255216640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-MX"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="251107920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2661,6 +3991,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3216,20 +4586,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>438149</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3243,6 +5129,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3514,10 +5430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53:I55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3525,29 +5441,30 @@
     <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -3555,1293 +5472,1745 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="G5" s="6" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="H5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F6" s="1" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="G7" s="1">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>35</v>
+      </c>
+      <c r="C7" s="7">
+        <v>35</v>
+      </c>
+      <c r="D7" s="7">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1">
         <v>45</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>35</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>0.85</v>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>14</v>
       </c>
-      <c r="B10" s="1">
-        <f>(G10*-A7)+A8</f>
-        <v>1.612222222222222</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="B10" s="7"/>
+      <c r="F10">
+        <f>B3-A10</f>
+        <v>49</v>
+      </c>
+      <c r="G10" s="1">
         <f>A10-63</f>
         <v>-49</v>
       </c>
-      <c r="G10" s="1">
-        <f>F10/G7</f>
+      <c r="H10" s="1">
+        <f>G10/H7</f>
         <v>-1.0888888888888888</v>
-      </c>
-      <c r="H10" s="1">
-        <v>-1</v>
       </c>
       <c r="I10" s="1">
         <v>-1</v>
       </c>
+      <c r="J10" s="1">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>16</v>
       </c>
-      <c r="B11" s="1">
-        <f>(G11*-A7)+A8</f>
-        <v>1.5811111111111111</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" ref="F11:F60" si="0">A11-63</f>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="F11">
+        <f>B3-A11</f>
+        <v>47</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" ref="G11:G60" si="0">A11-63</f>
         <v>-47</v>
       </c>
-      <c r="G11" s="1">
-        <f>F11/G7</f>
+      <c r="H11" s="1">
+        <f>G11/H7</f>
         <v>-1.0444444444444445</v>
-      </c>
-      <c r="H11" s="1">
-        <v>-1</v>
       </c>
       <c r="I11" s="1">
         <v>-1</v>
       </c>
+      <c r="J11" s="1">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>18</v>
       </c>
-      <c r="B12" s="1">
-        <f>(G12*-A7)+A8</f>
-        <v>1.5499999999999998</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="F12">
+        <f>B3-A12</f>
+        <v>45</v>
+      </c>
+      <c r="G12" s="1">
         <f t="shared" si="0"/>
         <v>-45</v>
       </c>
-      <c r="G12" s="1">
-        <f>F12/G7</f>
-        <v>-1</v>
-      </c>
       <c r="H12" s="1">
+        <f>G12/H7</f>
         <v>-1</v>
       </c>
       <c r="I12" s="1">
         <v>-1</v>
       </c>
+      <c r="J12" s="1">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>20</v>
       </c>
-      <c r="B13" s="1">
-        <f>(G13*-A7)+A8</f>
-        <v>1.5188888888888887</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="F13">
+        <f>B3-A13</f>
+        <v>43</v>
+      </c>
+      <c r="G13" s="1">
         <f t="shared" si="0"/>
         <v>-43</v>
       </c>
-      <c r="G13" s="1">
-        <f>F13/G7</f>
+      <c r="H13" s="1">
+        <f>G13/H7</f>
         <v>-0.9555555555555556</v>
-      </c>
-      <c r="H13" s="1">
-        <v>-1</v>
       </c>
       <c r="I13" s="1">
         <v>-1</v>
       </c>
+      <c r="J13" s="1">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>22</v>
       </c>
-      <c r="B14" s="1">
-        <f>(G14*-A7)+A8</f>
-        <v>1.4877777777777776</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="F14">
+        <f>B3-A14</f>
+        <v>41</v>
+      </c>
+      <c r="G14" s="1">
         <f t="shared" si="0"/>
         <v>-41</v>
       </c>
-      <c r="G14" s="1">
-        <f>F14/G7</f>
+      <c r="H14" s="1">
+        <f>G14/H7</f>
         <v>-0.91111111111111109</v>
-      </c>
-      <c r="H14" s="1">
-        <v>-1</v>
       </c>
       <c r="I14" s="1">
         <v>-1</v>
       </c>
+      <c r="J14" s="1">
+        <v>-1</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>24</v>
       </c>
-      <c r="B15" s="1">
-        <f>(G15*-A7)+A8</f>
-        <v>1.4566666666666666</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="B15" s="7">
+        <f>1-(F15/B7)</f>
+        <v>-0.11428571428571432</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="F15">
+        <f>B3-A15</f>
+        <v>39</v>
+      </c>
+      <c r="G15" s="1">
         <f t="shared" si="0"/>
         <v>-39</v>
       </c>
-      <c r="G15" s="1">
-        <f>F15/G7</f>
+      <c r="H15" s="1">
+        <f>G15/H7</f>
         <v>-0.8666666666666667</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>26</v>
       </c>
-      <c r="B16" s="1">
-        <f>(G16*-A7)+A8</f>
-        <v>1.4255555555555555</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="B16" s="7">
+        <f>1-(F16/B7)</f>
+        <v>-5.7142857142857162E-2</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="F16">
+        <f>B3-A16</f>
+        <v>37</v>
+      </c>
+      <c r="G16" s="1">
         <f t="shared" si="0"/>
         <v>-37</v>
       </c>
-      <c r="G16" s="1">
-        <f>F16/G7</f>
+      <c r="H16" s="1">
+        <f>G16/H7</f>
         <v>-0.82222222222222219</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>28</v>
       </c>
-      <c r="B17" s="1">
-        <f>(G17*-A7)+A8</f>
-        <v>1.3944444444444444</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="B17" s="7">
+        <f>1-(F17/B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="F17">
+        <f>B3-A17</f>
+        <v>35</v>
+      </c>
+      <c r="G17" s="1">
         <f t="shared" si="0"/>
         <v>-35</v>
       </c>
-      <c r="G17" s="1">
-        <f>F17/G7</f>
+      <c r="H17" s="1">
+        <f>G17/H7</f>
         <v>-0.77777777777777779</v>
       </c>
-      <c r="H17" s="1">
-        <f t="shared" ref="H17:H34" si="1">-1*(F17/35)^2</f>
+      <c r="I17" s="1">
+        <f t="shared" ref="I17:I34" si="1">-1*(G17/35)^2</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>30</v>
       </c>
-      <c r="B18" s="1">
-        <f>(G18*-A7)+A8</f>
-        <v>1.3633333333333333</v>
-      </c>
-      <c r="F18" s="1">
+      <c r="B18" s="7">
+        <f>1-(F18/B7)</f>
+        <v>5.7142857142857162E-2</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="F18">
+        <f>B3-A18</f>
+        <v>33</v>
+      </c>
+      <c r="G18" s="1">
         <f t="shared" si="0"/>
         <v>-33</v>
       </c>
-      <c r="G18" s="1">
-        <f>F18/G7</f>
+      <c r="H18" s="1">
+        <f>G18/H7</f>
         <v>-0.73333333333333328</v>
       </c>
-      <c r="H18" s="1">
-        <f t="shared" si="1"/>
+      <c r="I18" s="1">
+        <f>-1*(G18/35)^2</f>
         <v>-0.88897959183673469</v>
       </c>
-      <c r="I18" s="1">
-        <f>(F18/I7)^3</f>
+      <c r="J18" s="1">
+        <f>(G18/J7)^3</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>32</v>
       </c>
-      <c r="B19" s="1">
-        <f>(G19*-A7)+A8</f>
-        <v>1.3322222222222222</v>
-      </c>
-      <c r="F19" s="1">
+      <c r="B19" s="7">
+        <f>1-(F19/B7)</f>
+        <v>0.11428571428571432</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="F19">
+        <f>B3-A19</f>
+        <v>31</v>
+      </c>
+      <c r="G19" s="1">
         <f t="shared" si="0"/>
         <v>-31</v>
       </c>
-      <c r="G19" s="1">
-        <f>F19/G7</f>
+      <c r="H19" s="1">
+        <f>G19/H7</f>
         <v>-0.68888888888888888</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <f t="shared" si="1"/>
         <v>-0.78448979591836732</v>
       </c>
-      <c r="I19" s="1">
-        <f>(F19/I7)^3</f>
+      <c r="J19" s="1">
+        <f>(G19/J7)^3</f>
         <v>-0.82897849013551506</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>34</v>
       </c>
-      <c r="B20" s="1">
-        <f>(G20*-A7)+A8</f>
-        <v>1.3011111111111111</v>
-      </c>
-      <c r="F20" s="1">
+      <c r="B20" s="7">
+        <f>1-(F20/B7)</f>
+        <v>0.17142857142857137</v>
+      </c>
+      <c r="C20" s="7">
+        <f>1-((F20/C7)^2)</f>
+        <v>0.31346938775510191</v>
+      </c>
+      <c r="D20">
+        <f>1-((F20/D7)^3)</f>
+        <v>0.32134012299301562</v>
+      </c>
+      <c r="F20">
+        <f>B3-A20</f>
+        <v>29</v>
+      </c>
+      <c r="G20" s="1">
         <f t="shared" si="0"/>
         <v>-29</v>
       </c>
-      <c r="G20" s="1">
-        <f>F20/G7</f>
+      <c r="H20" s="1">
+        <f>G20/H7</f>
         <v>-0.64444444444444449</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <f t="shared" si="1"/>
         <v>-0.68653061224489809</v>
       </c>
-      <c r="I20" s="1">
-        <f>(F20/I7)^3</f>
+      <c r="J20" s="1">
+        <f>(G20/J7)^3</f>
         <v>-0.67865987700698438</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>36</v>
       </c>
-      <c r="B21" s="1">
-        <f>(G21*-A7)+A8</f>
-        <v>1.27</v>
-      </c>
-      <c r="F21" s="1">
+      <c r="B21" s="7">
+        <f>1-(F21/B7)</f>
+        <v>0.22857142857142854</v>
+      </c>
+      <c r="C21" s="7">
+        <f>1-((F21/C7)^2)</f>
+        <v>0.40489795918367344</v>
+      </c>
+      <c r="D21">
+        <f>1-((F21/D7)^3)</f>
+        <v>0.45229151014274971</v>
+      </c>
+      <c r="F21">
+        <f>B3-A21</f>
+        <v>27</v>
+      </c>
+      <c r="G21" s="1">
         <f t="shared" si="0"/>
         <v>-27</v>
       </c>
-      <c r="G21" s="1">
-        <f>F21/G7</f>
+      <c r="H21" s="1">
+        <f>G21/H7</f>
         <v>-0.6</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <f t="shared" si="1"/>
         <v>-0.59510204081632656</v>
       </c>
-      <c r="I21" s="1">
-        <f>(F21/I7)^3</f>
+      <c r="J21" s="1">
+        <f>(G21/J7)^3</f>
         <v>-0.54770848985725029</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>38</v>
       </c>
-      <c r="B22" s="1">
-        <f>(G22*-A7)+A8</f>
-        <v>1.2388888888888889</v>
-      </c>
-      <c r="F22" s="1">
+      <c r="B22" s="7">
+        <f>1-(F22/B7)</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="C22" s="7">
+        <f>1-((F22/C7)^2)</f>
+        <v>0.48979591836734693</v>
+      </c>
+      <c r="D22">
+        <f>1-((F22/D7)^3)</f>
+        <v>0.56521134207084622</v>
+      </c>
+      <c r="F22">
+        <f>B3-A22</f>
+        <v>25</v>
+      </c>
+      <c r="G22" s="1">
         <f t="shared" si="0"/>
         <v>-25</v>
       </c>
-      <c r="G22" s="1">
-        <f>F22/G7</f>
+      <c r="H22" s="1">
+        <f>G22/H7</f>
         <v>-0.55555555555555558</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <f t="shared" si="1"/>
         <v>-0.51020408163265307</v>
       </c>
-      <c r="I22" s="1">
-        <f>(F22/I7)^3</f>
+      <c r="J22" s="1">
+        <f>(G22/J7)^3</f>
         <v>-0.43478865792915378</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>40</v>
       </c>
-      <c r="B23" s="1">
-        <f>(G23*-A7)+A8</f>
-        <v>1.2077777777777778</v>
-      </c>
-      <c r="F23" s="1">
+      <c r="B23" s="7">
+        <f>1-(F23/B7)</f>
+        <v>0.34285714285714286</v>
+      </c>
+      <c r="C23" s="7">
+        <f>1-((F23/C7)^2)</f>
+        <v>0.56816326530612238</v>
+      </c>
+      <c r="D23">
+        <f>1-((F23/D7)^3)</f>
+        <v>0.66143528953446307</v>
+      </c>
+      <c r="F23">
+        <f>B3-A23</f>
+        <v>23</v>
+      </c>
+      <c r="G23" s="1">
         <f t="shared" si="0"/>
         <v>-23</v>
       </c>
-      <c r="G23" s="1">
-        <f>F23/G7</f>
+      <c r="H23" s="1">
+        <f>G23/H7</f>
         <v>-0.51111111111111107</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <f t="shared" si="1"/>
         <v>-0.43183673469387757</v>
       </c>
-      <c r="I23" s="1">
-        <f>(F23/I7)^3</f>
+      <c r="J23" s="1">
+        <f>(G23/J7)^3</f>
         <v>-0.33856471046553699</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42</v>
       </c>
-      <c r="B24" s="1">
-        <f>(G24*-A7)+A8</f>
-        <v>1.1766666666666667</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="B24" s="7">
+        <f>1-(F24/B7)</f>
+        <v>0.4</v>
+      </c>
+      <c r="C24" s="7">
+        <f>1-((F24/C7)^2)</f>
+        <v>0.64</v>
+      </c>
+      <c r="D24">
+        <f>1-((F24/D7)^3)</f>
+        <v>0.74229902329075892</v>
+      </c>
+      <c r="F24">
+        <f>B3-A24</f>
+        <v>21</v>
+      </c>
+      <c r="G24" s="1">
         <f t="shared" si="0"/>
         <v>-21</v>
       </c>
-      <c r="G24" s="1">
-        <f>F24/G7</f>
+      <c r="H24" s="1">
+        <f>G24/H7</f>
         <v>-0.46666666666666667</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <f t="shared" si="1"/>
         <v>-0.36</v>
       </c>
-      <c r="I24" s="1">
-        <f>(F24/I7)^3</f>
+      <c r="J24" s="1">
+        <f>(G24/J7)^3</f>
         <v>-0.25770097670924114</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44</v>
       </c>
-      <c r="B25" s="1">
-        <f>(G25*-A7)+A8</f>
-        <v>1.1455555555555554</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="B25" s="7">
+        <f>1-(F25/B7)</f>
+        <v>0.45714285714285718</v>
+      </c>
+      <c r="C25" s="7">
+        <f>1-((F25/C7)^2)</f>
+        <v>0.70530612244897961</v>
+      </c>
+      <c r="D25">
+        <f>1-((F25/D7)^3)</f>
+        <v>0.80913821409689168</v>
+      </c>
+      <c r="F25">
+        <f>B3-A25</f>
+        <v>19</v>
+      </c>
+      <c r="G25" s="1">
         <f t="shared" si="0"/>
         <v>-19</v>
       </c>
-      <c r="G25" s="1">
-        <f>F25/G7</f>
+      <c r="H25" s="1">
+        <f>G25/H7</f>
         <v>-0.42222222222222222</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <f t="shared" si="1"/>
         <v>-0.29469387755102039</v>
       </c>
-      <c r="I25" s="1">
-        <f>(F25/I7)^3</f>
+      <c r="J25" s="1">
+        <f>(G25/J7)^3</f>
         <v>-0.19086178590310826</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>46</v>
       </c>
-      <c r="B26" s="1">
-        <f>(G26*-A7)+A8</f>
-        <v>1.1144444444444443</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="B26" s="7">
+        <f>1-(F26/B7)</f>
+        <v>0.51428571428571423</v>
+      </c>
+      <c r="C26" s="7">
+        <f>1-((F26/C7)^2)</f>
+        <v>0.76408163265306128</v>
+      </c>
+      <c r="D26">
+        <f>1-((F26/D7)^3)</f>
+        <v>0.86328853271002037</v>
+      </c>
+      <c r="F26">
+        <f>B3-A26</f>
+        <v>17</v>
+      </c>
+      <c r="G26" s="1">
         <f t="shared" si="0"/>
         <v>-17</v>
       </c>
-      <c r="G26" s="1">
-        <f>F26/G7</f>
+      <c r="H26" s="1">
+        <f>G26/H7</f>
         <v>-0.37777777777777777</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <f t="shared" si="1"/>
         <v>-0.23591836734693877</v>
       </c>
-      <c r="I26" s="1">
-        <f>(F26/I7)^3</f>
+      <c r="J26" s="1">
+        <f>(G26/J7)^3</f>
         <v>-0.13671146728997968</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>48</v>
       </c>
-      <c r="B27" s="1">
-        <f>(G27*-A7)+A8</f>
-        <v>1.0833333333333333</v>
-      </c>
-      <c r="F27" s="1">
+      <c r="B27" s="7">
+        <f>1-(F27/B7)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="C27" s="7">
+        <f>1-((F27/C7)^2)</f>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="D27">
+        <f>1-((F27/D7)^3)</f>
+        <v>0.90608564988730278</v>
+      </c>
+      <c r="F27">
+        <f>B3-A27</f>
+        <v>15</v>
+      </c>
+      <c r="G27" s="1">
         <f t="shared" si="0"/>
         <v>-15</v>
       </c>
-      <c r="G27" s="1">
-        <f>F27/G7</f>
+      <c r="H27" s="1">
+        <f>G27/H7</f>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <f t="shared" si="1"/>
         <v>-0.18367346938775508</v>
       </c>
-      <c r="I27" s="1">
-        <f>(F27/I7)^3</f>
+      <c r="J27" s="1">
+        <f>(G27/J7)^3</f>
         <v>-9.3914350112697206E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>50</v>
       </c>
-      <c r="B28" s="1">
-        <f>(G28*-A7)+A8</f>
-        <v>1.0522222222222222</v>
-      </c>
-      <c r="F28" s="1">
+      <c r="B28" s="7">
+        <f>1-(F28/B7)</f>
+        <v>0.62857142857142856</v>
+      </c>
+      <c r="C28" s="7">
+        <f>1-((F28/C7)^2)</f>
+        <v>0.86204081632653062</v>
+      </c>
+      <c r="D28">
+        <f>1-((F28/D7)^3)</f>
+        <v>0.93886523638589758</v>
+      </c>
+      <c r="F28">
+        <f>B3-A28</f>
+        <v>13</v>
+      </c>
+      <c r="G28" s="1">
         <f t="shared" si="0"/>
         <v>-13</v>
       </c>
-      <c r="G28" s="1">
-        <f>F28/G7</f>
+      <c r="H28" s="1">
+        <f>G28/H7</f>
         <v>-0.28888888888888886</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <f t="shared" si="1"/>
         <v>-0.1379591836734694</v>
       </c>
-      <c r="I28" s="1">
-        <f>(F28/I7)^3</f>
+      <c r="J28" s="1">
+        <f>(G28/J7)^3</f>
         <v>-6.1134763614102451E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>52</v>
       </c>
-      <c r="B29" s="1">
-        <f>(G29*-A7)+A8</f>
-        <v>1.0211111111111111</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="B29" s="7">
+        <f>1-(F29/B7)</f>
+        <v>0.68571428571428572</v>
+      </c>
+      <c r="C29" s="7">
+        <f>1-((F29/C7)^2)</f>
+        <v>0.9012244897959184</v>
+      </c>
+      <c r="D29">
+        <f>1-((F29/D7)^3)</f>
+        <v>0.96296296296296302</v>
+      </c>
+      <c r="F29">
+        <f>B3-A29</f>
+        <v>11</v>
+      </c>
+      <c r="G29" s="1">
         <f t="shared" si="0"/>
         <v>-11</v>
       </c>
-      <c r="G29" s="1">
-        <f>F29/G7</f>
+      <c r="H29" s="1">
+        <f>G29/H7</f>
         <v>-0.24444444444444444</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <f t="shared" si="1"/>
         <v>-9.8775510204081624E-2</v>
       </c>
-      <c r="I29" s="1">
-        <f>(F29/I7)^3</f>
+      <c r="J29" s="1">
+        <f>(G29/J7)^3</f>
         <v>-3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>54</v>
       </c>
-      <c r="B30" s="1">
-        <f>(G30*-A7)+A8</f>
-        <v>0.99</v>
-      </c>
-      <c r="F30" s="1">
+      <c r="B30" s="7">
+        <f>1-(F30/B7)</f>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="C30" s="7">
+        <f>1-((F30/C7)^2)</f>
+        <v>0.93387755102040815</v>
+      </c>
+      <c r="D30">
+        <f>1-((F30/D7)^3)</f>
+        <v>0.97971450037565744</v>
+      </c>
+      <c r="F30">
+        <f>B3-A30</f>
+        <v>9</v>
+      </c>
+      <c r="G30" s="1">
         <f t="shared" si="0"/>
         <v>-9</v>
       </c>
-      <c r="G30" s="1">
-        <f>F30/G7</f>
+      <c r="H30" s="1">
+        <f>G30/H7</f>
         <v>-0.2</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <f t="shared" si="1"/>
         <v>-6.6122448979591825E-2</v>
       </c>
-      <c r="I30" s="1">
-        <f>(F30/I7)^3</f>
+      <c r="J30" s="1">
+        <f>(G30/J7)^3</f>
         <v>-2.0285499624342593E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>56</v>
       </c>
-      <c r="B31" s="1">
-        <f>(G31*-A7)+A8</f>
-        <v>0.9588888888888889</v>
-      </c>
-      <c r="F31" s="1">
+      <c r="B31" s="7">
+        <f>1-(F31/B7)</f>
+        <v>0.8</v>
+      </c>
+      <c r="C31" s="7">
+        <f>1-((F31/C7)^2)</f>
+        <v>0.96</v>
+      </c>
+      <c r="D31">
+        <f>1-((F31/D7)^3)</f>
+        <v>0.99045551938113918</v>
+      </c>
+      <c r="F31">
+        <f>B3-A31</f>
+        <v>7</v>
+      </c>
+      <c r="G31" s="1">
         <f t="shared" si="0"/>
         <v>-7</v>
       </c>
-      <c r="G31" s="1">
-        <f>F31/G7</f>
+      <c r="H31" s="1">
+        <f>G31/H7</f>
         <v>-0.15555555555555556</v>
       </c>
-      <c r="H31" s="1">
+      <c r="I31" s="1">
         <f t="shared" si="1"/>
         <v>-4.0000000000000008E-2</v>
       </c>
-      <c r="I31" s="1">
-        <f>(F31/I7)^3</f>
+      <c r="J31" s="1">
+        <f>(G31/J7)^3</f>
         <v>-9.5444806188607848E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>58</v>
       </c>
-      <c r="B32" s="1">
-        <f>(G32*-A7)+A8</f>
-        <v>0.9277777777777777</v>
-      </c>
-      <c r="F32" s="1">
+      <c r="B32" s="7">
+        <f>1-(F32/B7)</f>
+        <v>0.85714285714285721</v>
+      </c>
+      <c r="C32" s="7">
+        <f>1-((F32/C7)^2)</f>
+        <v>0.97959183673469385</v>
+      </c>
+      <c r="D32">
+        <f>1-((F32/D7)^3)</f>
+        <v>0.99652169073656682</v>
+      </c>
+      <c r="F32">
+        <f>B3-A32</f>
+        <v>5</v>
+      </c>
+      <c r="G32" s="1">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="G32" s="1">
-        <f>F32/G7</f>
+      <c r="H32" s="1">
+        <f>G32/H7</f>
         <v>-0.1111111111111111</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <f t="shared" si="1"/>
         <v>-2.0408163265306121E-2</v>
       </c>
-      <c r="I32" s="1">
-        <f>(F32/I7)^3</f>
+      <c r="J32" s="1">
+        <f>(G32/J7)^3</f>
         <v>-3.4783092634332307E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>60</v>
       </c>
-      <c r="B33" s="1">
-        <f>(G33*-A7)+A8</f>
-        <v>0.89666666666666661</v>
-      </c>
-      <c r="F33" s="1">
+      <c r="B33" s="7">
+        <f>1-(F33/B7)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="C33" s="7">
+        <f>1-((F33/C7)^2)</f>
+        <v>0.99265306122448982</v>
+      </c>
+      <c r="D33">
+        <f>1-((F33/D7)^3)</f>
+        <v>0.99924868519909837</v>
+      </c>
+      <c r="F33">
+        <f>B3-A33</f>
+        <v>3</v>
+      </c>
+      <c r="G33" s="1">
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="G33" s="1">
-        <f>F33/G7</f>
+      <c r="H33" s="1">
+        <f>G33/H7</f>
         <v>-6.6666666666666666E-2</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <f t="shared" si="1"/>
         <v>-7.3469387755102046E-3</v>
       </c>
-      <c r="I33" s="1">
-        <f>(F33/I7)^3</f>
+      <c r="J33" s="1">
+        <f>(G33/J7)^3</f>
         <v>-7.513148009015778E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>62</v>
       </c>
-      <c r="B34" s="1">
-        <f>(G34*-A7)+A8</f>
-        <v>0.86555555555555552</v>
-      </c>
-      <c r="F34" s="1">
+      <c r="B34" s="7">
+        <f>1-(F34/B7)</f>
+        <v>0.97142857142857142</v>
+      </c>
+      <c r="C34" s="7">
+        <f>1-((F34/C7)^2)</f>
+        <v>0.99918367346938775</v>
+      </c>
+      <c r="D34">
+        <f>1-((F34/D7)^3)</f>
+        <v>0.99997217352589252</v>
+      </c>
+      <c r="F34">
+        <f>B3-A34</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G34" s="1">
-        <f>F34/G7</f>
+      <c r="H34" s="1">
+        <f>G34/H7</f>
         <v>-2.2222222222222223E-2</v>
       </c>
-      <c r="H34" s="1">
+      <c r="I34" s="1">
         <f t="shared" si="1"/>
         <v>-8.1632653061224482E-4</v>
       </c>
-      <c r="I34" s="1">
-        <f>(F34/I7)^3</f>
+      <c r="J34" s="1">
+        <f>(G34/J7)^3</f>
         <v>-2.7826474107465846E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>63</v>
       </c>
-      <c r="B35" s="1">
-        <f>(G35*-A7)+A8</f>
-        <v>0.85</v>
-      </c>
-      <c r="F35" s="1">
+      <c r="B35" s="7">
+        <f>1-(F35/B7)</f>
+        <v>1</v>
+      </c>
+      <c r="C35" s="7">
+        <f>1-((F35/C7)^2)</f>
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <f>1-((F35/D7)^3)</f>
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <f>B3-A35</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G35" s="1">
-        <f>F35/G7</f>
+      <c r="H35" s="1">
+        <f>G35/H7</f>
         <v>0</v>
       </c>
-      <c r="H35" s="1">
-        <f t="shared" ref="H35:H52" si="2">(F35/35)^2</f>
+      <c r="I35" s="1">
+        <f t="shared" ref="I35:I52" si="2">(G35/35)^2</f>
         <v>0</v>
       </c>
-      <c r="I35" s="1">
-        <f>(F35/I7)^3</f>
+      <c r="J35" s="1">
+        <f>(G35/J7)^3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>64</v>
       </c>
-      <c r="B36" s="1">
-        <f>(G36*-A7)+A8</f>
-        <v>0.83444444444444443</v>
-      </c>
-      <c r="F36" s="1">
+      <c r="B36" s="7">
+        <f>1-(F36/B7)</f>
+        <v>0.97142857142857142</v>
+      </c>
+      <c r="C36" s="7">
+        <f>1-((F36/C7)^2)</f>
+        <v>0.99918367346938775</v>
+      </c>
+      <c r="D36">
+        <f>1-((F36/D7)^3)</f>
+        <v>0.99997217352589252</v>
+      </c>
+      <c r="F36">
+        <f>A36-B3</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G36" s="1">
-        <f>F36/G7</f>
+      <c r="H36" s="1">
+        <f>G36/H7</f>
         <v>2.2222222222222223E-2</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <f t="shared" si="2"/>
         <v>8.1632653061224482E-4</v>
       </c>
-      <c r="I36" s="1">
-        <f>(F36/I7)^3</f>
+      <c r="J36" s="1">
+        <f>(G36/J7)^3</f>
         <v>2.7826474107465846E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>66</v>
       </c>
-      <c r="B37" s="1">
-        <f>(G37*-A7)+A8</f>
-        <v>0.80333333333333334</v>
-      </c>
-      <c r="F37" s="1">
+      <c r="B37" s="7">
+        <f>1-(F37/B7)</f>
+        <v>0.91428571428571426</v>
+      </c>
+      <c r="C37" s="7">
+        <f>1-((F37/C7)^2)</f>
+        <v>0.99265306122448982</v>
+      </c>
+      <c r="D37">
+        <f>1-((F37/D7)^3)</f>
+        <v>0.99924868519909837</v>
+      </c>
+      <c r="F37">
+        <f>A37-B3</f>
+        <v>3</v>
+      </c>
+      <c r="G37" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G37" s="1">
-        <f>F37/G7</f>
+      <c r="H37" s="1">
+        <f>G37/H7</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="H37" s="1">
+      <c r="I37" s="1">
         <f t="shared" si="2"/>
         <v>7.3469387755102046E-3</v>
       </c>
-      <c r="I37" s="1">
-        <f>(F37/I7)^3</f>
+      <c r="J37" s="1">
+        <f>(G37/J7)^3</f>
         <v>7.513148009015778E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>68</v>
       </c>
-      <c r="B38" s="1">
-        <f>(G38*-A7)+A8</f>
-        <v>0.77222222222222225</v>
-      </c>
-      <c r="F38" s="1">
+      <c r="B38" s="7">
+        <f>1-(F38/B7)</f>
+        <v>0.85714285714285721</v>
+      </c>
+      <c r="C38" s="7">
+        <f>1-((F38/C7)^2)</f>
+        <v>0.97959183673469385</v>
+      </c>
+      <c r="D38">
+        <f>1-((F38/D7)^3)</f>
+        <v>0.99652169073656682</v>
+      </c>
+      <c r="F38">
+        <f>A38-B3</f>
+        <v>5</v>
+      </c>
+      <c r="G38" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G38" s="1">
-        <f>F38/G7</f>
+      <c r="H38" s="1">
+        <f>G38/H7</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="H38" s="1">
+      <c r="I38" s="1">
         <f t="shared" si="2"/>
         <v>2.0408163265306121E-2</v>
       </c>
-      <c r="I38" s="1">
-        <f>(F38/I7)^3</f>
+      <c r="J38" s="1">
+        <f>(G38/J7)^3</f>
         <v>3.4783092634332307E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>70</v>
       </c>
-      <c r="B39" s="1">
-        <f>(G39*-A7)+A8</f>
-        <v>0.74111111111111105</v>
-      </c>
-      <c r="F39" s="1">
+      <c r="B39" s="7">
+        <f>1-(F39/B7)</f>
+        <v>0.8</v>
+      </c>
+      <c r="C39" s="7">
+        <f>1-((F39/C7)^2)</f>
+        <v>0.96</v>
+      </c>
+      <c r="D39">
+        <f>1-((F39/D7)^3)</f>
+        <v>0.99045551938113918</v>
+      </c>
+      <c r="F39">
+        <f>A39-B3</f>
+        <v>7</v>
+      </c>
+      <c r="G39" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G39" s="1">
-        <f>F39/G7</f>
+      <c r="H39" s="1">
+        <f>G39/H7</f>
         <v>0.15555555555555556</v>
       </c>
-      <c r="H39" s="1">
+      <c r="I39" s="1">
         <f t="shared" si="2"/>
         <v>4.0000000000000008E-2</v>
       </c>
-      <c r="I39" s="1">
-        <f>(F39/40)^3</f>
+      <c r="J39" s="1">
+        <f>(G39/40)^3</f>
         <v>5.3593749999999987E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>72</v>
       </c>
-      <c r="B40" s="1">
-        <f>(G40*-A7)+A8</f>
-        <v>0.71</v>
-      </c>
-      <c r="F40" s="1">
+      <c r="B40" s="7">
+        <f>1-(F40/B7)</f>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="C40" s="7">
+        <f>1-((F40/C7)^2)</f>
+        <v>0.93387755102040815</v>
+      </c>
+      <c r="D40">
+        <f>1-((F40/D7)^3)</f>
+        <v>0.97971450037565744</v>
+      </c>
+      <c r="F40">
+        <f>A40-B3</f>
+        <v>9</v>
+      </c>
+      <c r="G40" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G40" s="1">
-        <f>F40/G7</f>
+      <c r="H40" s="1">
+        <f>G40/H7</f>
         <v>0.2</v>
       </c>
-      <c r="H40" s="1">
+      <c r="I40" s="1">
         <f t="shared" si="2"/>
         <v>6.6122448979591825E-2</v>
       </c>
-      <c r="I40" s="5">
-        <f>(F40/I7)^3</f>
+      <c r="J40" s="5">
+        <f>(G40/J7)^3</f>
         <v>2.0285499624342593E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>74</v>
       </c>
-      <c r="B41" s="1">
-        <f>(G41*-A7)+A8</f>
-        <v>0.67888888888888888</v>
-      </c>
-      <c r="F41" s="1">
+      <c r="B41" s="7">
+        <f>1-(F41/B7)</f>
+        <v>0.68571428571428572</v>
+      </c>
+      <c r="C41" s="7">
+        <f>1-((F41/C7)^2)</f>
+        <v>0.9012244897959184</v>
+      </c>
+      <c r="D41">
+        <f>1-((F41/D7)^3)</f>
+        <v>0.96296296296296302</v>
+      </c>
+      <c r="F41">
+        <f>A41-B3</f>
+        <v>11</v>
+      </c>
+      <c r="G41" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G41" s="1">
-        <f>F41/G7</f>
+      <c r="H41" s="1">
+        <f>G41/H7</f>
         <v>0.24444444444444444</v>
       </c>
-      <c r="H41" s="1">
+      <c r="I41" s="1">
         <f t="shared" si="2"/>
         <v>9.8775510204081624E-2</v>
       </c>
-      <c r="I41" s="1">
-        <f>(F41/I7)^3</f>
+      <c r="J41" s="1">
+        <f>(G41/J7)^3</f>
         <v>3.7037037037037035E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>76</v>
       </c>
-      <c r="B42" s="1">
-        <f>(G42*-A7)+A8</f>
-        <v>0.64777777777777779</v>
-      </c>
-      <c r="F42" s="1">
+      <c r="B42" s="7">
+        <f>1-(F42/B7)</f>
+        <v>0.62857142857142856</v>
+      </c>
+      <c r="C42" s="7">
+        <f>1-((F42/C7)^2)</f>
+        <v>0.86204081632653062</v>
+      </c>
+      <c r="D42">
+        <f>1-((F42/D7)^3)</f>
+        <v>0.93886523638589758</v>
+      </c>
+      <c r="F42">
+        <f>A42-B3</f>
+        <v>13</v>
+      </c>
+      <c r="G42" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G42" s="1">
-        <f>F42/G7</f>
+      <c r="H42" s="1">
+        <f>G42/H7</f>
         <v>0.28888888888888886</v>
       </c>
-      <c r="H42" s="1">
+      <c r="I42" s="1">
         <f t="shared" si="2"/>
         <v>0.1379591836734694</v>
       </c>
-      <c r="I42" s="1">
-        <f>(F42/I7)^3</f>
+      <c r="J42" s="1">
+        <f>(G42/J7)^3</f>
         <v>6.1134763614102451E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>78</v>
       </c>
-      <c r="B43" s="1">
-        <f>(G43*-A7)+A8</f>
-        <v>0.6166666666666667</v>
-      </c>
-      <c r="F43" s="1">
+      <c r="B43" s="7">
+        <f>1-(F43/B7)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="C43" s="7">
+        <f>1-((F43/C7)^2)</f>
+        <v>0.81632653061224492</v>
+      </c>
+      <c r="D43">
+        <f>1-((F43/D7)^3)</f>
+        <v>0.90608564988730278</v>
+      </c>
+      <c r="F43">
+        <f>A43-B3</f>
+        <v>15</v>
+      </c>
+      <c r="G43" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G43" s="1">
-        <f>F43/G7</f>
+      <c r="H43" s="1">
+        <f>G43/H7</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H43" s="1">
+      <c r="I43" s="1">
         <f t="shared" si="2"/>
         <v>0.18367346938775508</v>
       </c>
-      <c r="I43" s="1">
-        <f>(F43/I7)^3</f>
+      <c r="J43" s="1">
+        <f>(G43/J7)^3</f>
         <v>9.3914350112697206E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>80</v>
       </c>
-      <c r="B44" s="1">
-        <f>(G44*-A7)+A8</f>
-        <v>0.58555555555555561</v>
-      </c>
-      <c r="F44" s="1">
+      <c r="B44" s="7">
+        <f>1-(F44/B7)</f>
+        <v>0.51428571428571423</v>
+      </c>
+      <c r="C44" s="7">
+        <f>1-((F44/C7)^2)</f>
+        <v>0.76408163265306128</v>
+      </c>
+      <c r="D44">
+        <f>1-((F44/D7)^3)</f>
+        <v>0.86328853271002037</v>
+      </c>
+      <c r="F44">
+        <f>A44-B3</f>
+        <v>17</v>
+      </c>
+      <c r="G44" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G44" s="1">
-        <f>F44/G7</f>
+      <c r="H44" s="1">
+        <f>G44/H7</f>
         <v>0.37777777777777777</v>
       </c>
-      <c r="H44" s="1">
+      <c r="I44" s="1">
         <f t="shared" si="2"/>
         <v>0.23591836734693877</v>
       </c>
-      <c r="I44" s="1">
-        <f>(F44/I7)^3</f>
+      <c r="J44" s="1">
+        <f>(G44/J7)^3</f>
         <v>0.13671146728997968</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>82</v>
       </c>
-      <c r="B45" s="1">
-        <f>(G45*-A7)+A8</f>
-        <v>0.55444444444444452</v>
-      </c>
-      <c r="F45" s="1">
+      <c r="B45" s="7">
+        <f>1-(F45/B7)</f>
+        <v>0.45714285714285718</v>
+      </c>
+      <c r="C45" s="7">
+        <f>1-((F45/C7)^2)</f>
+        <v>0.70530612244897961</v>
+      </c>
+      <c r="D45">
+        <f>1-((F45/D7)^3)</f>
+        <v>0.80913821409689168</v>
+      </c>
+      <c r="F45">
+        <f>A45-B3</f>
+        <v>19</v>
+      </c>
+      <c r="G45" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="G45" s="1">
-        <f>F45/G7</f>
+      <c r="H45" s="1">
+        <f>G45/H7</f>
         <v>0.42222222222222222</v>
       </c>
-      <c r="H45" s="1">
+      <c r="I45" s="1">
         <f t="shared" si="2"/>
         <v>0.29469387755102039</v>
       </c>
-      <c r="I45" s="1">
-        <f>(F45/I7)^3</f>
+      <c r="J45" s="1">
+        <f>(G45/J7)^3</f>
         <v>0.19086178590310826</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>84</v>
       </c>
-      <c r="B46" s="1">
-        <f>(G46*-A7)+A8</f>
-        <v>0.52333333333333332</v>
-      </c>
-      <c r="F46" s="1">
+      <c r="B46" s="7">
+        <f>1-(F46/B7)</f>
+        <v>0.4</v>
+      </c>
+      <c r="C46" s="7">
+        <f>1-((F46/C7)^2)</f>
+        <v>0.64</v>
+      </c>
+      <c r="D46">
+        <f>1-((F46/D7)^3)</f>
+        <v>0.74229902329075892</v>
+      </c>
+      <c r="F46">
+        <f>A46-B3</f>
+        <v>21</v>
+      </c>
+      <c r="G46" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G46" s="1">
-        <f>F46/G7</f>
+      <c r="H46" s="1">
+        <f>G46/H7</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="H46" s="1">
+      <c r="I46" s="1">
         <f t="shared" si="2"/>
         <v>0.36</v>
       </c>
-      <c r="I46" s="1">
-        <f>(F46/I7)^3</f>
+      <c r="J46" s="1">
+        <f>(G46/J7)^3</f>
         <v>0.25770097670924114</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>86</v>
       </c>
-      <c r="B47" s="1">
-        <f>(G47*-A7)+A8</f>
-        <v>0.49222222222222223</v>
-      </c>
-      <c r="F47" s="1">
+      <c r="B47" s="7">
+        <f>1-(F47/B7)</f>
+        <v>0.34285714285714286</v>
+      </c>
+      <c r="C47" s="7">
+        <f>1-((F47/C7)^2)</f>
+        <v>0.56816326530612238</v>
+      </c>
+      <c r="D47">
+        <f>1-((F47/D7)^3)</f>
+        <v>0.66143528953446307</v>
+      </c>
+      <c r="F47">
+        <f>A47-B3</f>
+        <v>23</v>
+      </c>
+      <c r="G47" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G47" s="1">
-        <f>F47/G7</f>
+      <c r="H47" s="1">
+        <f>G47/H7</f>
         <v>0.51111111111111107</v>
       </c>
-      <c r="H47" s="1">
+      <c r="I47" s="1">
         <f t="shared" si="2"/>
         <v>0.43183673469387757</v>
       </c>
-      <c r="I47" s="1">
-        <f>(F47/I7)^3</f>
+      <c r="J47" s="1">
+        <f>(G47/J7)^3</f>
         <v>0.33856471046553699</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>88</v>
       </c>
-      <c r="B48" s="1">
-        <f>(G48*-A7)+A8</f>
-        <v>0.46111111111111108</v>
-      </c>
-      <c r="F48" s="1">
+      <c r="B48" s="7">
+        <f>1-(F48/B7)</f>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="C48" s="7">
+        <f>1-((F48/C7)^2)</f>
+        <v>0.48979591836734693</v>
+      </c>
+      <c r="D48">
+        <f>1-((F48/D7)^3)</f>
+        <v>0.56521134207084622</v>
+      </c>
+      <c r="F48">
+        <f>A48-B3</f>
+        <v>25</v>
+      </c>
+      <c r="G48" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G48" s="1">
-        <f>F48/G7</f>
+      <c r="H48" s="1">
+        <f>G48/H7</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="H48" s="1">
+      <c r="I48" s="1">
         <f t="shared" si="2"/>
         <v>0.51020408163265307</v>
       </c>
-      <c r="I48" s="1">
-        <f>(F48/I7)^3</f>
+      <c r="J48" s="1">
+        <f>(G48/J7)^3</f>
         <v>0.43478865792915378</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>90</v>
       </c>
-      <c r="B49" s="1">
-        <f>(G49*-A7)+A8</f>
-        <v>0.43</v>
-      </c>
-      <c r="F49" s="1">
+      <c r="B49" s="7">
+        <f>1-(F49/B7)</f>
+        <v>0.22857142857142854</v>
+      </c>
+      <c r="C49" s="7">
+        <f>1-((F49/C7)^2)</f>
+        <v>0.40489795918367344</v>
+      </c>
+      <c r="D49">
+        <f>1-((F49/D7)^3)</f>
+        <v>0.45229151014274971</v>
+      </c>
+      <c r="F49">
+        <f>A49-B3</f>
+        <v>27</v>
+      </c>
+      <c r="G49" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="G49" s="1">
-        <f>F49/G7</f>
+      <c r="H49" s="1">
+        <f>G49/H7</f>
         <v>0.6</v>
       </c>
-      <c r="H49" s="1">
+      <c r="I49" s="1">
         <f t="shared" si="2"/>
         <v>0.59510204081632656</v>
       </c>
-      <c r="I49" s="1">
-        <f>(F49/I7)^3</f>
+      <c r="J49" s="1">
+        <f>(G49/J7)^3</f>
         <v>0.54770848985725029</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>92</v>
       </c>
-      <c r="B50" s="1">
-        <f>(G50*-A7)+A8</f>
-        <v>0.39888888888888885</v>
-      </c>
-      <c r="F50" s="1">
+      <c r="B50" s="7">
+        <f>1-(F50/B7)</f>
+        <v>0.17142857142857137</v>
+      </c>
+      <c r="C50" s="7">
+        <f>1-((F50/C7)^2)</f>
+        <v>0.31346938775510191</v>
+      </c>
+      <c r="D50">
+        <f>1-((F50/D7)^3)</f>
+        <v>0.32134012299301562</v>
+      </c>
+      <c r="F50">
+        <f>A50-B3</f>
+        <v>29</v>
+      </c>
+      <c r="G50" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="G50" s="1">
-        <f>F50/G7</f>
+      <c r="H50" s="1">
+        <f>G50/H7</f>
         <v>0.64444444444444449</v>
       </c>
-      <c r="H50" s="1">
+      <c r="I50" s="1">
         <f t="shared" si="2"/>
         <v>0.68653061224489809</v>
       </c>
-      <c r="I50" s="1">
-        <f>(F50/I7)^3</f>
+      <c r="J50" s="1">
+        <f>(G50/J7)^3</f>
         <v>0.67865987700698438</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>94</v>
       </c>
-      <c r="B51" s="1">
-        <f>(G51*-A7)+A8</f>
-        <v>0.36777777777777781</v>
-      </c>
-      <c r="F51" s="1">
+      <c r="B51" s="7">
+        <f>1-(F51/B7)</f>
+        <v>0.11428571428571432</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="F51">
+        <f>A51-B3</f>
+        <v>31</v>
+      </c>
+      <c r="G51" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="G51" s="1">
-        <f>F51/G7</f>
+      <c r="H51" s="1">
+        <f>G51/H7</f>
         <v>0.68888888888888888</v>
       </c>
-      <c r="H51" s="1">
+      <c r="I51" s="1">
         <f t="shared" si="2"/>
         <v>0.78448979591836732</v>
       </c>
-      <c r="I51" s="1">
-        <f>(F51/I7)^3</f>
+      <c r="J51" s="1">
+        <f>(G51/J7)^3</f>
         <v>0.82897849013551506</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>96</v>
       </c>
-      <c r="B52" s="1">
-        <f>(G52*-A7)+A8</f>
-        <v>0.33666666666666667</v>
-      </c>
-      <c r="F52" s="1">
+      <c r="B52" s="7">
+        <f>1-(F52/B7)</f>
+        <v>5.7142857142857162E-2</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="F52">
+        <f>A52-B3</f>
+        <v>33</v>
+      </c>
+      <c r="G52" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="G52" s="1">
-        <f>F52/G7</f>
+      <c r="H52" s="1">
+        <f>G52/H7</f>
         <v>0.73333333333333328</v>
       </c>
-      <c r="H52" s="1">
+      <c r="I52" s="1">
         <f t="shared" si="2"/>
         <v>0.88897959183673469</v>
       </c>
-      <c r="I52" s="1">
-        <f>(F52/I7)^3</f>
+      <c r="J52" s="1">
+        <f>(G52/J7)^3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>98</v>
       </c>
-      <c r="B53" s="1">
-        <f>(G53*-A7)+A8</f>
-        <v>0.30555555555555558</v>
-      </c>
-      <c r="F53" s="1">
+      <c r="B53" s="7">
+        <f>1-(F53/B7)</f>
+        <v>0</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="F53">
+        <f>A53-B3</f>
+        <v>35</v>
+      </c>
+      <c r="G53" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="G53" s="1">
-        <f>F53/G7</f>
+      <c r="H53" s="1">
+        <f>G53/H7</f>
         <v>0.77777777777777779</v>
       </c>
-      <c r="H53" s="1">
-        <f t="shared" ref="H53" si="3">(F53/35)*(F53/35)</f>
+      <c r="I53" s="1">
+        <f t="shared" ref="I53" si="3">(G53/35)*(G53/35)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>100</v>
       </c>
-      <c r="B54" s="1">
-        <f>(G54*-A7)+A8</f>
-        <v>0.27444444444444449</v>
-      </c>
-      <c r="F54" s="1">
+      <c r="B54" s="7">
+        <f>1-(F54/B7)</f>
+        <v>-5.7142857142857162E-2</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="F54">
+        <f>A54-B3</f>
+        <v>37</v>
+      </c>
+      <c r="G54" s="1">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="G54" s="1">
-        <f>F54/G7</f>
+      <c r="H54" s="1">
+        <f>G54/H7</f>
         <v>0.82222222222222219</v>
       </c>
-      <c r="H54" s="1">
+      <c r="I54" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>102</v>
       </c>
-      <c r="B55" s="1">
-        <f>(G55*-A7)+A8</f>
-        <v>0.24333333333333329</v>
-      </c>
-      <c r="F55" s="1">
+      <c r="B55" s="7">
+        <f>1-(F55/B7)</f>
+        <v>-0.11428571428571432</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="F55">
+        <f>A55-B3</f>
+        <v>39</v>
+      </c>
+      <c r="G55" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="G55" s="1">
-        <f>F55/G7</f>
+      <c r="H55" s="1">
+        <f>G55/H7</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="H55" s="1">
+      <c r="I55" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>104</v>
       </c>
-      <c r="B56" s="1">
-        <f>(G56*-A7)+A8</f>
-        <v>0.2122222222222222</v>
-      </c>
-      <c r="F56" s="1">
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="F56">
+        <f>A56-B3</f>
+        <v>41</v>
+      </c>
+      <c r="G56" s="1">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="G56" s="1">
-        <f>F56/G7</f>
+      <c r="H56" s="1">
+        <f>G56/H7</f>
         <v>0.91111111111111109</v>
-      </c>
-      <c r="H56" s="1">
-        <v>1</v>
       </c>
       <c r="I56" s="1">
         <v>1</v>
       </c>
+      <c r="J56" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>106</v>
       </c>
-      <c r="B57" s="1">
-        <f>(G57*-A7)+A8</f>
-        <v>0.18111111111111111</v>
-      </c>
-      <c r="F57" s="1">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="F57">
+        <f>A57-B3</f>
+        <v>43</v>
+      </c>
+      <c r="G57" s="1">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="G57" s="1">
-        <f>F57/G7</f>
+      <c r="H57" s="1">
+        <f>G57/H7</f>
         <v>0.9555555555555556</v>
-      </c>
-      <c r="H57" s="1">
-        <v>1</v>
       </c>
       <c r="I57" s="1">
         <v>1</v>
       </c>
+      <c r="J57" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>108</v>
       </c>
-      <c r="B58" s="1">
-        <f>(G58*-A7)+A8</f>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="F58" s="1">
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="F58">
+        <f>A58-B3</f>
+        <v>45</v>
+      </c>
+      <c r="G58" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="G58" s="1">
-        <f>F58/G7</f>
-        <v>1</v>
-      </c>
       <c r="H58" s="1">
+        <f>G58/H7</f>
         <v>1</v>
       </c>
       <c r="I58" s="1">
         <v>1</v>
       </c>
+      <c r="J58" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>110</v>
       </c>
-      <c r="B59" s="1">
-        <f>(G59*-A7)+A8</f>
-        <v>0.11888888888888882</v>
-      </c>
-      <c r="F59" s="1">
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="F59">
+        <f>A59-B3</f>
+        <v>47</v>
+      </c>
+      <c r="G59" s="1">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="G59" s="1">
-        <f>F59/G7</f>
+      <c r="H59" s="1">
+        <f>G59/H7</f>
         <v>1.0444444444444445</v>
-      </c>
-      <c r="H59" s="1">
-        <v>1</v>
       </c>
       <c r="I59" s="1">
         <v>1</v>
       </c>
+      <c r="J59" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>112</v>
       </c>
-      <c r="B60" s="1">
-        <f>(G60*-A7)+A8</f>
-        <v>8.7777777777777843E-2</v>
-      </c>
-      <c r="F60" s="1">
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="F60">
+        <f>A60-B3</f>
+        <v>49</v>
+      </c>
+      <c r="G60" s="1">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="G60" s="1">
-        <f>F60/G7</f>
+      <c r="H60" s="1">
+        <f>G60/H7</f>
         <v>1.0888888888888888</v>
       </c>
-      <c r="H60" s="1">
+      <c r="I60" s="1">
         <v>1</v>
       </c>
-      <c r="I60" s="1">
+      <c r="J60" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4867,20 +7236,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -4921,7 +7290,7 @@
       <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E5">
@@ -4950,7 +7319,7 @@
       <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="11"/>
       <c r="E6">
         <v>0.4</v>
       </c>
@@ -4977,7 +7346,7 @@
       <c r="C7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="11"/>
       <c r="E7">
         <v>0.4</v>
       </c>
@@ -5004,7 +7373,7 @@
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="11"/>
       <c r="E8">
         <v>0.4</v>
       </c>
@@ -5029,7 +7398,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E10">
@@ -5053,7 +7422,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="9"/>
+      <c r="D11" s="11"/>
       <c r="E11">
         <v>0.4</v>
       </c>
@@ -5075,7 +7444,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="9"/>
+      <c r="D12" s="11"/>
       <c r="E12">
         <v>0.4</v>
       </c>
@@ -5097,7 +7466,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="11"/>
       <c r="E13">
         <v>0.4</v>
       </c>

</xml_diff>